<commit_message>
Set up Team Tab
</commit_message>
<xml_diff>
--- a/TeamDRAINReport.xlsx
+++ b/TeamDRAINReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16098\Documents\CS555\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanqin/Desktop/SSW555_DRAIN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{479DAB71-9B03-4504-B4A8-6772E4003271}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250A6052-89F3-EE4A-900C-2D69A32F831E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="240">
   <si>
     <t>Find marriage date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -240,9 +240,6 @@
     <t>Bring silverware for everyone</t>
   </si>
   <si>
-    <t>ssw555tmxx2015Fall</t>
-  </si>
-  <si>
     <t>Dates (birth, marriage, divorce, death) should not be after the current date</t>
   </si>
   <si>
@@ -795,7 +792,19 @@
     <t>Miah</t>
   </si>
   <si>
-    <t>nh</t>
+    <t>rqin@stevens.edu</t>
+  </si>
+  <si>
+    <t>nmiah@stevens.edu</t>
+  </si>
+  <si>
+    <t>agomes@stevens.edu</t>
+  </si>
+  <si>
+    <t>rqin00</t>
+  </si>
+  <si>
+    <t>SSW555_DRAIN</t>
   </si>
 </sst>
 </file>
@@ -1090,7 +1099,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1161,7 +1170,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2135,19 +2144,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.453125" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" customWidth="1"/>
-    <col min="4" max="5" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -2164,85 +2173,97 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" t="s">
         <v>215</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>216</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="19" t="s">
         <v>217</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="E2" t="s">
         <v>218</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>220</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>221</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="E3" t="s">
         <v>223</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="E4" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>233</v>
-      </c>
-      <c r="B4" t="s">
-        <v>234</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C5" t="s">
+        <v>228</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="E5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6" t="s">
+        <v>230</v>
+      </c>
+      <c r="C6" t="s">
+        <v>231</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="E4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>227</v>
-      </c>
-      <c r="B5" t="s">
-        <v>228</v>
-      </c>
-      <c r="C5" t="s">
-        <v>229</v>
-      </c>
-      <c r="E5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>230</v>
-      </c>
-      <c r="B6" t="s">
-        <v>231</v>
-      </c>
-      <c r="C6" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2253,6 +2274,9 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{703C676E-B8F2-435C-88A3-3D40894F017F}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{DAEF2113-B5C7-4D08-AE42-DA899A5CA48B}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{B4C9A7A1-1246-FA47-A90C-8E0632CFE79D}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{720CEDB6-2B34-0B41-A22D-446D59A21DB2}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{3B21B841-9FA2-2244-94B4-99E4D642A9C4}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2267,16 +2291,16 @@
       <selection activeCell="D2" sqref="D2:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" customWidth="1"/>
-    <col min="3" max="3" width="19.453125" customWidth="1"/>
-    <col min="4" max="4" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
@@ -2293,37 +2317,37 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2341,49 +2365,49 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="7"/>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="7" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="7" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="4" t="s">
         <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>182</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>3</v>
@@ -2404,9 +2428,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B15" s="13">
         <v>41065</v>
@@ -2420,9 +2444,9 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B16" s="13">
         <v>41078</v>
@@ -2445,9 +2469,9 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B17" s="13">
         <v>41092</v>
@@ -2470,9 +2494,9 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B18" s="13">
         <v>41106</v>
@@ -2495,9 +2519,9 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B19" s="13">
         <v>41120</v>
@@ -2535,17 +2559,17 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="2"/>
-    <col min="2" max="2" width="16.6328125" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="7.1796875" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -2565,7 +2589,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>42406</v>
       </c>
@@ -2576,7 +2600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B3">
         <v>40</v>
       </c>
@@ -2607,31 +2631,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.453125" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.81640625" style="17" customWidth="1"/>
-    <col min="15" max="15" width="10.1796875" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.453125" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.83203125" style="17" customWidth="1"/>
+    <col min="15" max="15" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -2660,30 +2684,30 @@
         <v>20</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L1" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="M1" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="O1" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="P1" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="O1" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="P1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="Q1" s="16" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
@@ -2707,27 +2731,27 @@
         <v>40444</v>
       </c>
       <c r="K2" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="L2" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="M2" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="M2" s="18" t="s">
-        <v>202</v>
-      </c>
       <c r="O2" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P2" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q2" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="Q2" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>38</v>
@@ -2736,9 +2760,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>39</v>
@@ -2747,9 +2771,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>40</v>
@@ -2758,12 +2782,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
         <v>32</v>
@@ -2778,27 +2802,27 @@
         <v>120</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L8" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="M8" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="O8" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="P8" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="M8" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="O8" s="18" t="s">
-        <v>214</v>
-      </c>
-      <c r="P8" s="18" t="s">
+      <c r="Q8" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="Q8" s="18" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>42</v>
@@ -2810,9 +2834,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>0</v>
@@ -2821,9 +2845,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
@@ -2832,36 +2856,36 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" ht="28" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" ht="28" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" ht="28" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
         <v>49</v>
       </c>
@@ -2878,15 +2902,15 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="27.26953125" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -2915,114 +2939,114 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
         <v>129</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23" t="s">
         <v>177</v>
       </c>
-      <c r="C2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>131</v>
-      </c>
-      <c r="B8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>132</v>
-      </c>
-      <c r="B11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>133</v>
-      </c>
-      <c r="B14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C14" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>134</v>
-      </c>
-      <c r="B17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C17" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>135</v>
-      </c>
-      <c r="B20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="C23" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
         <v>136</v>
       </c>
-      <c r="B23" t="s">
-        <v>178</v>
-      </c>
-      <c r="C23" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
         <v>137</v>
       </c>
-      <c r="B26" t="s">
-        <v>91</v>
-      </c>
-      <c r="C26" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>138</v>
-      </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C29" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -3040,9 +3064,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -3085,13 +3109,13 @@
       <selection activeCell="A2" sqref="A2:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="27.7265625" customWidth="1"/>
-    <col min="3" max="3" width="31.36328125" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -3120,31 +3144,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C2" s="12"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C3" s="12"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C4" s="12"/>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C5" s="12"/>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C6" s="12"/>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C9" s="12"/>
     </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C10" s="12"/>
     </row>
   </sheetData>
@@ -3161,483 +3185,483 @@
       <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C4" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="12" t="s">
+      <c r="C9" s="12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>136</v>
-      </c>
-      <c r="B9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>137</v>
-      </c>
-      <c r="B10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>138</v>
-      </c>
-      <c r="B11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="12" t="s">
+    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>139</v>
-      </c>
-      <c r="B12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="12" t="s">
+    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" t="s">
+        <v>190</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>140</v>
-      </c>
-      <c r="B13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>141</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C16" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" t="s">
+        <v>197</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>148</v>
+      </c>
+      <c r="B22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>150</v>
+      </c>
+      <c r="B24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>151</v>
+      </c>
+      <c r="B25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>142</v>
-      </c>
-      <c r="B15" t="s">
-        <v>191</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>143</v>
-      </c>
-      <c r="B16" t="s">
-        <v>98</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>144</v>
-      </c>
-      <c r="B17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>145</v>
-      </c>
-      <c r="B18" t="s">
-        <v>198</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>146</v>
-      </c>
-      <c r="B19" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>147</v>
-      </c>
-      <c r="B20" t="s">
-        <v>101</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>148</v>
-      </c>
-      <c r="B21" t="s">
-        <v>102</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>149</v>
-      </c>
-      <c r="B22" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>150</v>
-      </c>
-      <c r="B23" t="s">
-        <v>106</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>151</v>
-      </c>
-      <c r="B24" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>152</v>
-      </c>
-      <c r="B25" t="s">
-        <v>108</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>153</v>
-      </c>
-      <c r="B26" t="s">
-        <v>109</v>
-      </c>
-      <c r="C26" s="12" t="s">
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>154</v>
-      </c>
-      <c r="B27" t="s">
-        <v>110</v>
-      </c>
-      <c r="C27" s="12" t="s">
+    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>155</v>
-      </c>
-      <c r="B28" t="s">
-        <v>111</v>
-      </c>
-      <c r="C28" s="12" t="s">
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>156</v>
+      </c>
+      <c r="B30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="12" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>156</v>
-      </c>
-      <c r="B29" t="s">
-        <v>112</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
         <v>157</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>113</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C31" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
         <v>158</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>114</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C32" s="12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
         <v>159</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>115</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C33" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
         <v>160</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>116</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C34" s="12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
         <v>161</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
+        <v>126</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>162</v>
+      </c>
+      <c r="B36" t="s">
         <v>117</v>
       </c>
-      <c r="C34" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>162</v>
-      </c>
-      <c r="B35" t="s">
-        <v>127</v>
-      </c>
-      <c r="C35" s="12" t="s">
+      <c r="C36" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
         <v>163</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>118</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C37" s="12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
         <v>164</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>119</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C38" s="12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
         <v>165</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>120</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C39" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
         <v>166</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>121</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C40" s="12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
         <v>167</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>122</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C41" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>168</v>
+      </c>
+      <c r="B42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>168</v>
-      </c>
-      <c r="B41" t="s">
-        <v>123</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
         <v>169</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>125</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C43" s="12" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>170</v>
-      </c>
-      <c r="B43" t="s">
-        <v>126</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Sprint 1 again
</commit_message>
<xml_diff>
--- a/TeamDRAINReport.xlsx
+++ b/TeamDRAINReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agome\Documents\GitHub\SSW555_DRAIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0814AD-9413-4D6F-868D-C3AC2D2DB354}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE989DAF-38C9-4849-A2BD-13901B15A401}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="239">
   <si>
     <t>Find marriage date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -130,10 +130,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Story Name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -178,10 +174,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Story ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Owner</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -807,6 +799,9 @@
   </si>
   <si>
     <t>SSW555_DRAIN</t>
+  </si>
+  <si>
+    <t>Assigned</t>
   </si>
 </sst>
 </file>
@@ -2160,112 +2155,112 @@
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" t="s">
         <v>214</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>216</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" t="s">
         <v>219</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>221</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="E3" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B4" t="s">
+        <v>231</v>
+      </c>
+      <c r="C4" t="s">
         <v>232</v>
       </c>
-      <c r="B4" t="s">
-        <v>233</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>236</v>
-      </c>
       <c r="E4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C5" t="s">
         <v>226</v>
       </c>
-      <c r="B5" t="s">
-        <v>227</v>
-      </c>
-      <c r="C5" t="s">
-        <v>228</v>
-      </c>
       <c r="D5" s="19" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B6" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" t="s">
         <v>229</v>
       </c>
-      <c r="B6" t="s">
-        <v>230</v>
-      </c>
-      <c r="C6" t="s">
-        <v>231</v>
-      </c>
       <c r="D6" s="19" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2287,36 +2282,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E4"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" customWidth="1"/>
-    <col min="3" max="3" width="19.453125" customWidth="1"/>
+    <col min="3" max="3" width="28.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.6328125" customWidth="1"/>
     <col min="5" max="5" width="7.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2324,10 +2318,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>83</v>
+        <v>126</v>
+      </c>
+      <c r="C2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E2" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2335,21 +2335,408 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>86</v>
+        <v>127</v>
+      </c>
+      <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E3" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>217</v>
+      </c>
+      <c r="E4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>230</v>
+      </c>
+      <c r="E7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" t="s">
+        <v>227</v>
+      </c>
+      <c r="E8" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" t="s">
+        <v>224</v>
+      </c>
+      <c r="E9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" t="s">
+        <v>224</v>
+      </c>
+      <c r="E10" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
         <v>135</v>
       </c>
-      <c r="C4" t="s">
-        <v>84</v>
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" t="s">
+        <v>227</v>
+      </c>
+      <c r="E11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>148</v>
+      </c>
+      <c r="C24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>149</v>
+      </c>
+      <c r="C25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>150</v>
+      </c>
+      <c r="C26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>151</v>
+      </c>
+      <c r="C27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>153</v>
+      </c>
+      <c r="C29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>154</v>
+      </c>
+      <c r="C30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>155</v>
+      </c>
+      <c r="C31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>156</v>
+      </c>
+      <c r="C32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>157</v>
+      </c>
+      <c r="C33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>158</v>
+      </c>
+      <c r="C34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>159</v>
+      </c>
+      <c r="C35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>160</v>
+      </c>
+      <c r="C36" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>161</v>
+      </c>
+      <c r="C37" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>162</v>
+      </c>
+      <c r="C38" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>163</v>
+      </c>
+      <c r="C39" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C40" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>165</v>
+      </c>
+      <c r="C41" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>166</v>
+      </c>
+      <c r="C42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2379,37 +2766,37 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>3</v>
@@ -2421,18 +2808,18 @@
         <v>5</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B15" s="13">
         <v>41065</v>
@@ -2448,7 +2835,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B16" s="13">
         <v>41078</v>
@@ -2473,7 +2860,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B17" s="13">
         <v>41092</v>
@@ -2498,7 +2885,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B18" s="13">
         <v>41106</v>
@@ -2523,7 +2910,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B19" s="13">
         <v>41120</v>
@@ -2582,13 +2969,13 @@
         <v>5</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2686,36 +3073,36 @@
         <v>20</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="L1" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="P1" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>204</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E2">
         <v>150</v>
@@ -2733,69 +3120,69 @@
         <v>40444</v>
       </c>
       <c r="K2" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="M2" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="L2" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>201</v>
-      </c>
       <c r="O2" s="18" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E8">
         <v>200</v>
@@ -2804,33 +3191,33 @@
         <v>120</v>
       </c>
       <c r="K8" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="M8" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="L8" s="18" t="s">
+      <c r="O8" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="P8" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q8" s="18" t="s">
         <v>209</v>
-      </c>
-      <c r="M8" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="O8" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="P8" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q8" s="18" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
@@ -2838,29 +3225,29 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -2869,27 +3256,27 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2903,8 +3290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2943,13 +3330,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E2">
         <v>30</v>
@@ -2960,57 +3347,81 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>219</v>
+        <v>217</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>219</v>
+        <v>217</v>
+      </c>
+      <c r="E8">
+        <v>30</v>
+      </c>
+      <c r="F8">
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>214</v>
+        <v>212</v>
+      </c>
+      <c r="E11">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C14" t="s">
-        <v>214</v>
+        <v>212</v>
+      </c>
+      <c r="E14">
+        <v>20</v>
+      </c>
+      <c r="F14">
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E17">
         <v>30</v>
@@ -3021,58 +3432,70 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C20" t="s">
-        <v>229</v>
+        <v>227</v>
+      </c>
+      <c r="E20">
+        <v>20</v>
+      </c>
+      <c r="F20">
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C23" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E23">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F23">
-        <v>120</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E26">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F26">
-        <v>120</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C29" t="s">
-        <v>229</v>
+        <v>227</v>
+      </c>
+      <c r="E29">
+        <v>30</v>
+      </c>
+      <c r="F29">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3207,8 +3630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B11"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3219,475 +3642,475 @@
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B30" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B34" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B36" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B37" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B38" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B39" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B40" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B41" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B42" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B43" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deleted file with error
</commit_message>
<xml_diff>
--- a/TeamDRAINReport.xlsx
+++ b/TeamDRAINReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agome\Documents\GitHub\SSW555_DRAIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0814AD-9413-4D6F-868D-C3AC2D2DB354}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A510DEF1-4A4E-4255-BA9A-DD7CF0331774}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="239">
   <si>
     <t>Find marriage date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -130,10 +130,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Story Name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Initials</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -178,10 +174,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Story ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Owner</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -807,6 +799,9 @@
   </si>
   <si>
     <t>SSW555_DRAIN</t>
+  </si>
+  <si>
+    <t>Assigned</t>
   </si>
 </sst>
 </file>
@@ -2160,112 +2155,112 @@
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" t="s">
         <v>214</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>216</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="E2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" t="s">
         <v>219</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>221</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="E3" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B4" t="s">
+        <v>231</v>
+      </c>
+      <c r="C4" t="s">
         <v>232</v>
       </c>
-      <c r="B4" t="s">
-        <v>233</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="D4" s="19" t="s">
-        <v>236</v>
-      </c>
       <c r="E4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C5" t="s">
         <v>226</v>
       </c>
-      <c r="B5" t="s">
-        <v>227</v>
-      </c>
-      <c r="C5" t="s">
-        <v>228</v>
-      </c>
       <c r="D5" s="19" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B6" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" t="s">
         <v>229</v>
       </c>
-      <c r="B6" t="s">
-        <v>230</v>
-      </c>
-      <c r="C6" t="s">
-        <v>231</v>
-      </c>
       <c r="D6" s="19" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2287,36 +2282,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E4"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" customWidth="1"/>
-    <col min="3" max="3" width="19.453125" customWidth="1"/>
+    <col min="3" max="3" width="28.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.6328125" customWidth="1"/>
     <col min="5" max="5" width="7.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2324,10 +2318,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>83</v>
+        <v>126</v>
+      </c>
+      <c r="C2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E2" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2335,21 +2335,408 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>86</v>
+        <v>127</v>
+      </c>
+      <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E3" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>217</v>
+      </c>
+      <c r="E4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>230</v>
+      </c>
+      <c r="E7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" t="s">
+        <v>227</v>
+      </c>
+      <c r="E8" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" t="s">
+        <v>224</v>
+      </c>
+      <c r="E9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" t="s">
+        <v>224</v>
+      </c>
+      <c r="E10" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
         <v>135</v>
       </c>
-      <c r="C4" t="s">
-        <v>84</v>
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" t="s">
+        <v>227</v>
+      </c>
+      <c r="E11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>148</v>
+      </c>
+      <c r="C24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>149</v>
+      </c>
+      <c r="C25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>150</v>
+      </c>
+      <c r="C26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>151</v>
+      </c>
+      <c r="C27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>153</v>
+      </c>
+      <c r="C29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>154</v>
+      </c>
+      <c r="C30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>155</v>
+      </c>
+      <c r="C31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>156</v>
+      </c>
+      <c r="C32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>157</v>
+      </c>
+      <c r="C33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>158</v>
+      </c>
+      <c r="C34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>159</v>
+      </c>
+      <c r="C35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>160</v>
+      </c>
+      <c r="C36" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>161</v>
+      </c>
+      <c r="C37" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>162</v>
+      </c>
+      <c r="C38" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>163</v>
+      </c>
+      <c r="C39" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C40" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>165</v>
+      </c>
+      <c r="C41" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>166</v>
+      </c>
+      <c r="C42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2379,37 +2766,37 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>3</v>
@@ -2421,18 +2808,18 @@
         <v>5</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B15" s="13">
         <v>41065</v>
@@ -2448,7 +2835,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B16" s="13">
         <v>41078</v>
@@ -2473,7 +2860,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B17" s="13">
         <v>41092</v>
@@ -2498,7 +2885,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B18" s="13">
         <v>41106</v>
@@ -2523,7 +2910,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B19" s="13">
         <v>41120</v>
@@ -2582,13 +2969,13 @@
         <v>5</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2686,36 +3073,36 @@
         <v>20</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="L1" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="P1" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>204</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E2">
         <v>150</v>
@@ -2733,69 +3120,69 @@
         <v>40444</v>
       </c>
       <c r="K2" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="M2" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="L2" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>201</v>
-      </c>
       <c r="O2" s="18" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E8">
         <v>200</v>
@@ -2804,33 +3191,33 @@
         <v>120</v>
       </c>
       <c r="K8" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="M8" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="L8" s="18" t="s">
+      <c r="O8" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="P8" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q8" s="18" t="s">
         <v>209</v>
-      </c>
-      <c r="M8" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="O8" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="P8" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q8" s="18" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
@@ -2838,29 +3225,29 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -2869,27 +3256,27 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2903,8 +3290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2943,13 +3330,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E2">
         <v>30</v>
@@ -2960,57 +3347,81 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>219</v>
+        <v>217</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>219</v>
+        <v>217</v>
+      </c>
+      <c r="E8">
+        <v>30</v>
+      </c>
+      <c r="F8">
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>214</v>
+        <v>212</v>
+      </c>
+      <c r="E11">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C14" t="s">
-        <v>214</v>
+        <v>212</v>
+      </c>
+      <c r="E14">
+        <v>20</v>
+      </c>
+      <c r="F14">
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E17">
         <v>30</v>
@@ -3021,58 +3432,70 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C20" t="s">
-        <v>229</v>
+        <v>227</v>
+      </c>
+      <c r="E20">
+        <v>20</v>
+      </c>
+      <c r="F20">
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C23" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E23">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F23">
-        <v>120</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E26">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F26">
-        <v>120</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C29" t="s">
-        <v>229</v>
+        <v>227</v>
+      </c>
+      <c r="E29">
+        <v>30</v>
+      </c>
+      <c r="F29">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3207,8 +3630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B11"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3219,475 +3642,475 @@
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B30" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B34" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B36" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B37" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B38" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B39" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B40" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B41" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B42" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B43" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed User Story 10
</commit_message>
<xml_diff>
--- a/TeamDRAINReport.xlsx
+++ b/TeamDRAINReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanqin/Desktop/SSW555_DRAIN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98756A5E-6143-5344-9C74-83DBE08A23A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FE4E25-E17B-7149-ADB9-BE4A043AEEB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19240" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="240">
   <si>
     <t>Find marriage date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -804,7 +804,7 @@
     <t>Assigned</t>
   </si>
   <si>
-    <t>Done</t>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -3295,7 +3295,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3454,7 +3454,7 @@
         <v>30</v>
       </c>
       <c r="G20">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H20">
         <v>31</v>
@@ -3507,11 +3507,23 @@
       <c r="C29" t="s">
         <v>227</v>
       </c>
+      <c r="D29" t="s">
+        <v>239</v>
+      </c>
       <c r="E29">
         <v>30</v>
       </c>
       <c r="F29">
         <v>45</v>
+      </c>
+      <c r="G29">
+        <v>17</v>
+      </c>
+      <c r="H29">
+        <v>23</v>
+      </c>
+      <c r="I29" s="20">
+        <v>42418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed User Stories with tests and updated excel sheet
</commit_message>
<xml_diff>
--- a/TeamDRAINReport.xlsx
+++ b/TeamDRAINReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanqin/Desktop/SSW555_DRAIN/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\SSW555_DRAIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FE4E25-E17B-7149-ADB9-BE4A043AEEB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B36791-D161-4A1F-9BF9-FE6D52A6CA54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19240" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="259">
   <si>
     <t>Find marriage date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -804,7 +804,64 @@
     <t>Assigned</t>
   </si>
   <si>
-    <t>Testing</t>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>parseGEDCOM.py</t>
+  </si>
+  <si>
+    <t>checkUS07</t>
+  </si>
+  <si>
+    <t>checkUS08</t>
+  </si>
+  <si>
+    <t>checkUS09</t>
+  </si>
+  <si>
+    <t>checkUS10</t>
+  </si>
+  <si>
+    <t>27-44</t>
+  </si>
+  <si>
+    <t>47-73</t>
+  </si>
+  <si>
+    <t>75-100</t>
+  </si>
+  <si>
+    <t>102-120</t>
+  </si>
+  <si>
+    <t>testUS07.py</t>
+  </si>
+  <si>
+    <t>testUS08.py</t>
+  </si>
+  <si>
+    <t>testUS09.py</t>
+  </si>
+  <si>
+    <t>testUS10.py</t>
+  </si>
+  <si>
+    <t>testUS07</t>
+  </si>
+  <si>
+    <t>testUS08</t>
+  </si>
+  <si>
+    <t>testUS09</t>
+  </si>
+  <si>
+    <t>testUS10</t>
+  </si>
+  <si>
+    <t>5-6</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -953,7 +1010,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -991,6 +1048,8 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="65"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1100,7 +1159,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1171,7 +1230,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1242,6 +1301,9 @@
                 <c:pt idx="0">
                   <c:v>42406</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>42419</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1255,7 +1317,7 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2149,15 +2211,15 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>21</v>
       </c>
@@ -2174,7 +2236,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>212</v>
       </c>
@@ -2191,7 +2253,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>217</v>
       </c>
@@ -2208,7 +2270,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>230</v>
       </c>
@@ -2225,7 +2287,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>224</v>
       </c>
@@ -2242,7 +2304,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>227</v>
       </c>
@@ -2259,7 +2321,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>45</v>
       </c>
@@ -2288,19 +2350,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" customWidth="1"/>
-    <col min="3" max="3" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" customWidth="1"/>
+    <col min="3" max="3" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>35</v>
       </c>
@@ -2317,7 +2379,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2334,7 +2396,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2351,7 +2413,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2368,7 +2430,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2385,7 +2447,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2402,7 +2464,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2419,7 +2481,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2433,10 +2495,10 @@
         <v>227</v>
       </c>
       <c r="E8" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2450,10 +2512,10 @@
         <v>224</v>
       </c>
       <c r="E9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2467,10 +2529,10 @@
         <v>224</v>
       </c>
       <c r="E10" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2484,10 +2546,10 @@
         <v>227</v>
       </c>
       <c r="E11" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>136</v>
       </c>
@@ -2495,7 +2557,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>137</v>
       </c>
@@ -2503,7 +2565,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>138</v>
       </c>
@@ -2511,7 +2573,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>139</v>
       </c>
@@ -2519,7 +2581,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>140</v>
       </c>
@@ -2527,7 +2589,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>141</v>
       </c>
@@ -2535,7 +2597,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>142</v>
       </c>
@@ -2543,7 +2605,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>143</v>
       </c>
@@ -2551,7 +2613,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>144</v>
       </c>
@@ -2559,7 +2621,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>145</v>
       </c>
@@ -2567,7 +2629,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>146</v>
       </c>
@@ -2575,7 +2637,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>147</v>
       </c>
@@ -2583,7 +2645,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>148</v>
       </c>
@@ -2591,7 +2653,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>149</v>
       </c>
@@ -2599,7 +2661,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>150</v>
       </c>
@@ -2607,7 +2669,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>151</v>
       </c>
@@ -2615,7 +2677,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>152</v>
       </c>
@@ -2623,7 +2685,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>153</v>
       </c>
@@ -2631,7 +2693,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>154</v>
       </c>
@@ -2639,7 +2701,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>155</v>
       </c>
@@ -2647,7 +2709,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>156</v>
       </c>
@@ -2655,7 +2717,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>157</v>
       </c>
@@ -2663,7 +2725,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>158</v>
       </c>
@@ -2671,7 +2733,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>159</v>
       </c>
@@ -2679,7 +2741,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>160</v>
       </c>
@@ -2687,7 +2749,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>161</v>
       </c>
@@ -2695,7 +2757,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>162</v>
       </c>
@@ -2703,7 +2765,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>163</v>
       </c>
@@ -2711,7 +2773,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>164</v>
       </c>
@@ -2719,7 +2781,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>165</v>
       </c>
@@ -2727,7 +2789,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>166</v>
       </c>
@@ -2735,7 +2797,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>167</v>
       </c>
@@ -2758,47 +2820,47 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="7"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>179</v>
       </c>
@@ -2821,7 +2883,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>180</v>
       </c>
@@ -2837,7 +2899,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>181</v>
       </c>
@@ -2862,7 +2924,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>182</v>
       </c>
@@ -2887,7 +2949,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>183</v>
       </c>
@@ -2912,7 +2974,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>184</v>
       </c>
@@ -2949,20 +3011,20 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="2"/>
+    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -2982,7 +3044,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>42406</v>
       </c>
@@ -2993,13 +3055,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>42419</v>
+      </c>
       <c r="B3">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <f>B2-B3</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>250</v>
@@ -3024,31 +3089,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1796875" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.83203125" style="17" customWidth="1"/>
-    <col min="15" max="15" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.81640625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="10.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1796875" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -3095,7 +3160,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -3142,7 +3207,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>168</v>
       </c>
@@ -3153,7 +3218,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>169</v>
       </c>
@@ -3164,7 +3229,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="28" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>170</v>
       </c>
@@ -3175,7 +3240,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>130</v>
       </c>
@@ -3213,7 +3278,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="28" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>171</v>
       </c>
@@ -3227,7 +3292,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>172</v>
       </c>
@@ -3238,7 +3303,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="28" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>173</v>
       </c>
@@ -3249,36 +3314,36 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="28" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="28" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="28" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>47</v>
       </c>
@@ -3292,18 +3357,33 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView zoomScale="93" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.36328125" customWidth="1"/>
+    <col min="3" max="3" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6328125" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2" customWidth="1"/>
+    <col min="15" max="15" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -3331,8 +3411,27 @@
       <c r="I1" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="K1" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="N1" s="17"/>
+      <c r="O1" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>126</v>
       </c>
@@ -3348,8 +3447,33 @@
       <c r="F2">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -3365,8 +3489,33 @@
       <c r="F5">
         <v>90</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -3382,8 +3531,15 @@
       <c r="F8">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>129</v>
       </c>
@@ -3400,7 +3556,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>130</v>
       </c>
@@ -3417,7 +3573,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>131</v>
       </c>
@@ -3434,7 +3590,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -3454,16 +3610,34 @@
         <v>30</v>
       </c>
       <c r="G20">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H20">
         <v>31</v>
       </c>
       <c r="I20" s="20">
-        <v>42418</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+        <v>42419</v>
+      </c>
+      <c r="K20" t="s">
+        <v>240</v>
+      </c>
+      <c r="L20" t="s">
+        <v>241</v>
+      </c>
+      <c r="M20" t="s">
+        <v>245</v>
+      </c>
+      <c r="O20" t="s">
+        <v>249</v>
+      </c>
+      <c r="P20" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q20" s="21" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>133</v>
       </c>
@@ -3473,14 +3647,44 @@
       <c r="C23" t="s">
         <v>224</v>
       </c>
+      <c r="D23" t="s">
+        <v>239</v>
+      </c>
       <c r="E23">
         <v>30</v>
       </c>
       <c r="F23">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G23">
+        <v>27</v>
+      </c>
+      <c r="H23">
+        <v>87</v>
+      </c>
+      <c r="I23" s="20">
+        <v>42419</v>
+      </c>
+      <c r="K23" t="s">
+        <v>240</v>
+      </c>
+      <c r="L23" t="s">
+        <v>242</v>
+      </c>
+      <c r="M23" t="s">
+        <v>246</v>
+      </c>
+      <c r="O23" t="s">
+        <v>250</v>
+      </c>
+      <c r="P23" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q23" s="22" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>134</v>
       </c>
@@ -3490,14 +3694,44 @@
       <c r="C26" t="s">
         <v>224</v>
       </c>
+      <c r="D26" t="s">
+        <v>239</v>
+      </c>
       <c r="E26">
         <v>30</v>
       </c>
       <c r="F26">
         <v>100</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G26">
+        <v>26</v>
+      </c>
+      <c r="H26">
+        <v>73</v>
+      </c>
+      <c r="I26" s="20">
+        <v>42419</v>
+      </c>
+      <c r="K26" t="s">
+        <v>240</v>
+      </c>
+      <c r="L26" t="s">
+        <v>243</v>
+      </c>
+      <c r="M26" t="s">
+        <v>247</v>
+      </c>
+      <c r="O26" t="s">
+        <v>251</v>
+      </c>
+      <c r="P26" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q26" s="22" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>135</v>
       </c>
@@ -3517,19 +3751,37 @@
         <v>45</v>
       </c>
       <c r="G29">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H29">
         <v>23</v>
       </c>
       <c r="I29" s="20">
-        <v>42418</v>
+        <v>42419</v>
+      </c>
+      <c r="K29" t="s">
+        <v>240</v>
+      </c>
+      <c r="L29" t="s">
+        <v>244</v>
+      </c>
+      <c r="M29" t="s">
+        <v>248</v>
+      </c>
+      <c r="O29" t="s">
+        <v>252</v>
+      </c>
+      <c r="P29" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q29" s="22" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3541,9 +3793,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -3586,13 +3838,13 @@
       <selection activeCell="A2" sqref="A2:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.6328125" customWidth="1"/>
+    <col min="3" max="3" width="31.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -3621,31 +3873,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="12"/>
     </row>
-    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C3" s="12"/>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C4" s="12"/>
     </row>
-    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C5" s="12"/>
     </row>
-    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C6" s="12"/>
     </row>
-    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C9" s="12"/>
     </row>
-    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C10" s="12"/>
     </row>
   </sheetData>
@@ -3662,13 +3914,13 @@
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>125</v>
       </c>
@@ -3679,7 +3931,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>126</v>
       </c>
@@ -3690,7 +3942,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -3701,7 +3953,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -3712,7 +3964,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -3723,7 +3975,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>130</v>
       </c>
@@ -3734,7 +3986,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>131</v>
       </c>
@@ -3745,7 +3997,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>132</v>
       </c>
@@ -3756,7 +4008,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>133</v>
       </c>
@@ -3767,7 +4019,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -3778,7 +4030,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>135</v>
       </c>
@@ -3789,7 +4041,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>136</v>
       </c>
@@ -3800,7 +4052,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>137</v>
       </c>
@@ -3811,7 +4063,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>138</v>
       </c>
@@ -3822,7 +4074,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>139</v>
       </c>
@@ -3833,7 +4085,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>140</v>
       </c>
@@ -3844,7 +4096,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>141</v>
       </c>
@@ -3855,7 +4107,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>142</v>
       </c>
@@ -3866,7 +4118,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>143</v>
       </c>
@@ -3877,7 +4129,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>144</v>
       </c>
@@ -3888,7 +4140,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>145</v>
       </c>
@@ -3899,7 +4151,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>146</v>
       </c>
@@ -3910,7 +4162,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>147</v>
       </c>
@@ -3921,7 +4173,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>148</v>
       </c>
@@ -3932,7 +4184,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>149</v>
       </c>
@@ -3943,7 +4195,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>150</v>
       </c>
@@ -3954,7 +4206,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>151</v>
       </c>
@@ -3965,7 +4217,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>152</v>
       </c>
@@ -3976,7 +4228,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>153</v>
       </c>
@@ -3987,7 +4239,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>154</v>
       </c>
@@ -3998,7 +4250,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>155</v>
       </c>
@@ -4009,7 +4261,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>156</v>
       </c>
@@ -4020,7 +4272,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>157</v>
       </c>
@@ -4031,7 +4283,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>158</v>
       </c>
@@ -4042,7 +4294,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>159</v>
       </c>
@@ -4053,7 +4305,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>160</v>
       </c>
@@ -4064,7 +4316,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>161</v>
       </c>
@@ -4075,7 +4327,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>162</v>
       </c>
@@ -4086,7 +4338,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>163</v>
       </c>
@@ -4097,7 +4349,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>164</v>
       </c>
@@ -4108,7 +4360,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>165</v>
       </c>
@@ -4119,7 +4371,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>166</v>
       </c>
@@ -4130,7 +4382,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>167</v>
       </c>

</xml_diff>

<commit_message>
completed US04 and US05
</commit_message>
<xml_diff>
--- a/TeamDRAINReport.xlsx
+++ b/TeamDRAINReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lieju\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16098\Desktop\SSW555_DRAIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FBB42C-2E88-45BE-A28B-00D23D533277}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B06E72-6497-44B6-AE90-4163BB9E086B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="282">
   <si>
     <t>Find marriage date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -801,9 +801,6 @@
     <t>SSW555_DRAIN</t>
   </si>
   <si>
-    <t>Assigned</t>
-  </si>
-  <si>
     <t>Done</t>
   </si>
   <si>
@@ -822,18 +819,6 @@
     <t>checkUS10</t>
   </si>
   <si>
-    <t>27-44</t>
-  </si>
-  <si>
-    <t>47-73</t>
-  </si>
-  <si>
-    <t>75-100</t>
-  </si>
-  <si>
-    <t>102-120</t>
-  </si>
-  <si>
     <t>testUS07.py</t>
   </si>
   <si>
@@ -870,12 +855,6 @@
     <t>checkUS03</t>
   </si>
   <si>
-    <t>51-64</t>
-  </si>
-  <si>
-    <t>27-48</t>
-  </si>
-  <si>
     <t>testUS02.py</t>
   </si>
   <si>
@@ -909,7 +888,49 @@
     <t>27-59</t>
   </si>
   <si>
-    <t>102-124</t>
+    <t>checkUS04</t>
+  </si>
+  <si>
+    <t>checkUS05</t>
+  </si>
+  <si>
+    <t>102-115</t>
+  </si>
+  <si>
+    <t>119-140</t>
+  </si>
+  <si>
+    <t>testUS04.py</t>
+  </si>
+  <si>
+    <t>testUS05.py</t>
+  </si>
+  <si>
+    <t>testUS04</t>
+  </si>
+  <si>
+    <t>testUS05</t>
+  </si>
+  <si>
+    <t>143-165</t>
+  </si>
+  <si>
+    <t>168-185</t>
+  </si>
+  <si>
+    <t>188-214</t>
+  </si>
+  <si>
+    <t>216-247</t>
+  </si>
+  <si>
+    <t>250-275</t>
+  </si>
+  <si>
+    <t>86-99</t>
+  </si>
+  <si>
+    <t>62-83</t>
   </si>
 </sst>
 </file>
@@ -1356,6 +1377,9 @@
                 <c:pt idx="1">
                   <c:v>42419</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>42422</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1370,6 +1394,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2263,12 +2290,12 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2403,15 +2430,15 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.125" customWidth="1"/>
-    <col min="3" max="3" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.625" customWidth="1"/>
-    <col min="5" max="5" width="9.625" customWidth="1"/>
+    <col min="1" max="1" width="5.08984375" customWidth="1"/>
+    <col min="3" max="3" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2445,7 +2472,7 @@
         <v>230</v>
       </c>
       <c r="E2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2462,7 +2489,7 @@
         <v>217</v>
       </c>
       <c r="E3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2479,7 +2506,7 @@
         <v>217</v>
       </c>
       <c r="E4" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2496,7 +2523,7 @@
         <v>212</v>
       </c>
       <c r="E5" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2513,7 +2540,7 @@
         <v>212</v>
       </c>
       <c r="E6" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2530,7 +2557,7 @@
         <v>230</v>
       </c>
       <c r="E7" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2547,7 +2574,7 @@
         <v>227</v>
       </c>
       <c r="E8" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2564,7 +2591,7 @@
         <v>224</v>
       </c>
       <c r="E9" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2581,7 +2608,7 @@
         <v>224</v>
       </c>
       <c r="E10" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2598,7 +2625,7 @@
         <v>227</v>
       </c>
       <c r="E11" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2872,14 +2899,14 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="7"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="7"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -3060,20 +3087,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="2"/>
+    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="7.08984375" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -3103,7 +3130,16 @@
       <c r="B2">
         <v>40</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
       <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9">
         <v>0</v>
       </c>
     </row>
@@ -3127,6 +3163,27 @@
       <c r="F3" s="9">
         <f>(D3-D2)/E3*60</f>
         <v>125.00000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>42422</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>450</v>
+      </c>
+      <c r="E4">
+        <v>436</v>
+      </c>
+      <c r="F4" s="9">
+        <f>D4/E4 * 60</f>
+        <v>61.926605504587151</v>
       </c>
     </row>
   </sheetData>
@@ -3145,24 +3202,24 @@
       <selection activeCell="K1" sqref="K1:Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.625" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.125" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.08984375" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.875" style="17" customWidth="1"/>
-    <col min="15" max="15" width="10.125" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.125" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.90625" style="17" customWidth="1"/>
+    <col min="15" max="15" width="10.08984375" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.08984375" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
@@ -3281,7 +3338,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>170</v>
       </c>
@@ -3330,7 +3387,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>171</v>
       </c>
@@ -3355,7 +3412,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>173</v>
       </c>
@@ -3385,7 +3442,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>48</v>
       </c>
@@ -3395,7 +3452,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>47</v>
       </c>
@@ -3409,30 +3466,30 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.375" customWidth="1"/>
-    <col min="3" max="3" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.625" customWidth="1"/>
-    <col min="5" max="5" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.36328125" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6328125" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="2" customWidth="1"/>
-    <col min="15" max="15" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
@@ -3494,7 +3551,7 @@
         <v>230</v>
       </c>
       <c r="D2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E2">
         <v>30</v>
@@ -3512,23 +3569,23 @@
         <v>42422</v>
       </c>
       <c r="K2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="N2" s="17"/>
       <c r="O2" s="18" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="P2" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="Q2" s="24" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -3575,23 +3632,23 @@
         <v>42421</v>
       </c>
       <c r="K5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L5" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
       <c r="N5" s="17"/>
       <c r="O5" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="P5" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="Q5" s="21" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -3638,23 +3695,23 @@
         <v>42421</v>
       </c>
       <c r="K8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L8" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="M8" s="18" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
       <c r="N8" s="17"/>
       <c r="O8" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="P8" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="Q8" s="21" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -3667,11 +3724,41 @@
       <c r="C11" t="s">
         <v>212</v>
       </c>
+      <c r="D11" t="s">
+        <v>238</v>
+      </c>
       <c r="E11">
         <v>20</v>
       </c>
       <c r="F11">
         <v>60</v>
+      </c>
+      <c r="G11">
+        <v>13</v>
+      </c>
+      <c r="H11">
+        <v>30</v>
+      </c>
+      <c r="I11" s="20">
+        <v>42422</v>
+      </c>
+      <c r="K11" t="s">
+        <v>239</v>
+      </c>
+      <c r="L11" t="s">
+        <v>267</v>
+      </c>
+      <c r="M11" t="s">
+        <v>269</v>
+      </c>
+      <c r="O11" t="s">
+        <v>271</v>
+      </c>
+      <c r="P11" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q11" s="20">
+        <v>42495</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
@@ -3684,11 +3771,41 @@
       <c r="C14" t="s">
         <v>212</v>
       </c>
+      <c r="D14" t="s">
+        <v>238</v>
+      </c>
       <c r="E14">
         <v>20</v>
       </c>
       <c r="F14">
         <v>60</v>
+      </c>
+      <c r="G14">
+        <v>21</v>
+      </c>
+      <c r="H14">
+        <v>40</v>
+      </c>
+      <c r="I14" s="20">
+        <v>42422</v>
+      </c>
+      <c r="K14" t="s">
+        <v>239</v>
+      </c>
+      <c r="L14" t="s">
+        <v>268</v>
+      </c>
+      <c r="M14" t="s">
+        <v>270</v>
+      </c>
+      <c r="O14" t="s">
+        <v>272</v>
+      </c>
+      <c r="P14" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q14" s="20">
+        <v>42495</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
@@ -3717,22 +3834,22 @@
         <v>42422</v>
       </c>
       <c r="K17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L17" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="M17" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="O17" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="P17" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="Q17" s="23" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
@@ -3746,7 +3863,7 @@
         <v>227</v>
       </c>
       <c r="D20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E20">
         <v>20</v>
@@ -3764,22 +3881,22 @@
         <v>42419</v>
       </c>
       <c r="K20" t="s">
+        <v>239</v>
+      </c>
+      <c r="L20" t="s">
         <v>240</v>
       </c>
-      <c r="L20" t="s">
-        <v>241</v>
-      </c>
       <c r="M20" t="s">
-        <v>245</v>
+        <v>276</v>
       </c>
       <c r="O20" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="P20" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="Q20" s="21" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
@@ -3793,7 +3910,7 @@
         <v>224</v>
       </c>
       <c r="D23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E23">
         <v>30</v>
@@ -3811,22 +3928,22 @@
         <v>42419</v>
       </c>
       <c r="K23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M23" t="s">
-        <v>246</v>
+        <v>277</v>
       </c>
       <c r="O23" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="P23" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="Q23" s="22" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
@@ -3840,7 +3957,7 @@
         <v>224</v>
       </c>
       <c r="D26" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E26">
         <v>30</v>
@@ -3858,22 +3975,22 @@
         <v>42419</v>
       </c>
       <c r="K26" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M26" t="s">
-        <v>247</v>
+        <v>278</v>
       </c>
       <c r="O26" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="P26" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="Q26" s="22" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
@@ -3887,7 +4004,7 @@
         <v>227</v>
       </c>
       <c r="D29" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E29">
         <v>30</v>
@@ -3905,22 +4022,28 @@
         <v>42419</v>
       </c>
       <c r="K29" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L29" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M29" t="s">
-        <v>248</v>
+        <v>279</v>
       </c>
       <c r="O29" t="s">
+        <v>247</v>
+      </c>
+      <c r="P29" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q29" s="22" t="s">
         <v>252</v>
       </c>
-      <c r="P29" t="s">
-        <v>256</v>
-      </c>
-      <c r="Q29" s="22" t="s">
-        <v>257</v>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H34">
+        <f>SUM(H2:H29)</f>
+        <v>436</v>
       </c>
     </row>
   </sheetData>
@@ -3934,13 +4057,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="G3" zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -3983,10 +4106,10 @@
       <selection activeCell="A2" sqref="A2:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.625" customWidth="1"/>
-    <col min="3" max="3" width="31.375" customWidth="1"/>
+    <col min="2" max="2" width="27.6328125" customWidth="1"/>
+    <col min="3" max="3" width="31.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -4018,31 +4141,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="12"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C3" s="12"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C4" s="12"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C5" s="12"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C6" s="12"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C9" s="12"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="C10" s="12"/>
     </row>
   </sheetData>
@@ -4059,10 +4182,10 @@
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4076,7 +4199,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>126</v>
       </c>
@@ -4087,7 +4210,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -4098,7 +4221,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -4109,7 +4232,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -4120,7 +4243,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>130</v>
       </c>
@@ -4131,7 +4254,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>131</v>
       </c>
@@ -4142,7 +4265,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>132</v>
       </c>
@@ -4153,7 +4276,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>133</v>
       </c>
@@ -4164,7 +4287,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -4175,7 +4298,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>135</v>
       </c>
@@ -4186,7 +4309,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>136</v>
       </c>
@@ -4197,7 +4320,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>137</v>
       </c>
@@ -4208,7 +4331,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>138</v>
       </c>
@@ -4219,7 +4342,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>139</v>
       </c>
@@ -4230,7 +4353,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>140</v>
       </c>
@@ -4241,7 +4364,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>141</v>
       </c>
@@ -4252,7 +4375,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>142</v>
       </c>
@@ -4263,7 +4386,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>143</v>
       </c>
@@ -4274,7 +4397,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>144</v>
       </c>
@@ -4285,7 +4408,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>145</v>
       </c>
@@ -4296,7 +4419,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>146</v>
       </c>
@@ -4307,7 +4430,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>147</v>
       </c>
@@ -4318,7 +4441,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>148</v>
       </c>
@@ -4329,7 +4452,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>149</v>
       </c>
@@ -4340,7 +4463,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>150</v>
       </c>
@@ -4351,7 +4474,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>151</v>
       </c>
@@ -4362,7 +4485,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>152</v>
       </c>
@@ -4373,7 +4496,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>153</v>
       </c>
@@ -4384,7 +4507,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>154</v>
       </c>
@@ -4395,7 +4518,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>155</v>
       </c>
@@ -4406,7 +4529,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>156</v>
       </c>
@@ -4417,7 +4540,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>157</v>
       </c>
@@ -4428,7 +4551,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>158</v>
       </c>
@@ -4439,7 +4562,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>159</v>
       </c>
@@ -4450,7 +4573,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>160</v>
       </c>
@@ -4461,7 +4584,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>161</v>
       </c>
@@ -4472,7 +4595,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>162</v>
       </c>
@@ -4483,7 +4606,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>163</v>
       </c>
@@ -4494,7 +4617,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>164</v>
       </c>
@@ -4505,7 +4628,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>165</v>
       </c>
@@ -4516,7 +4639,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>166</v>
       </c>
@@ -4527,7 +4650,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>167</v>
       </c>

</xml_diff>

<commit_message>
updated sprint planning log for team meeting
</commit_message>
<xml_diff>
--- a/TeamDRAINReport.xlsx
+++ b/TeamDRAINReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16098\Desktop\SSW555_DRAIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B06E72-6497-44B6-AE90-4163BB9E086B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E0D10B-26B0-4FF8-BDA9-62AF6E196A00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Burndown" sheetId="7" r:id="rId4"/>
     <sheet name="sample sprint" sheetId="3" r:id="rId5"/>
     <sheet name="Sprint1" sheetId="4" r:id="rId6"/>
-    <sheet name="Sprint3" sheetId="5" r:id="rId7"/>
+    <sheet name="Sprint2" sheetId="5" r:id="rId7"/>
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="309">
   <si>
     <t>Find marriage date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -931,6 +931,87 @@
   </si>
   <si>
     <t>62-83</t>
+  </si>
+  <si>
+    <t>dates- marriage</t>
+  </si>
+  <si>
+    <t>age, family members</t>
+  </si>
+  <si>
+    <t>dates- birth, family members</t>
+  </si>
+  <si>
+    <t>family members</t>
+  </si>
+  <si>
+    <t>marriage, family members</t>
+  </si>
+  <si>
+    <t>ids</t>
+  </si>
+  <si>
+    <t>name, dates- birth</t>
+  </si>
+  <si>
+    <t>name, dates- marriage</t>
+  </si>
+  <si>
+    <t>name, dates- birth, family members</t>
+  </si>
+  <si>
+    <t>ids, family members</t>
+  </si>
+  <si>
+    <t>dates- birth</t>
+  </si>
+  <si>
+    <t>dates- death</t>
+  </si>
+  <si>
+    <t>dates- marriage, dates- death</t>
+  </si>
+  <si>
+    <t>dates- death, dates- birth, family members</t>
+  </si>
+  <si>
+    <t>dates- birth, dates- marriage</t>
+  </si>
+  <si>
+    <t>dates- death, family members</t>
+  </si>
+  <si>
+    <t>misc</t>
+  </si>
+  <si>
+    <t>dates- all</t>
+  </si>
+  <si>
+    <t>Keep Doing:</t>
+  </si>
+  <si>
+    <t>Est Size</t>
+  </si>
+  <si>
+    <t>Doing things last-minute</t>
+  </si>
+  <si>
+    <t>More team meetings (virtual or in person)</t>
+  </si>
+  <si>
+    <t>Pair programming</t>
+  </si>
+  <si>
+    <t>Getting user stories done on time</t>
+  </si>
+  <si>
+    <t>Forgetting to comment code</t>
+  </si>
+  <si>
+    <t>Not double checking code</t>
+  </si>
+  <si>
+    <t>Assigned</t>
   </si>
 </sst>
 </file>
@@ -988,7 +1069,7 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -998,6 +1079,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1079,7 +1166,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1123,6 +1210,11 @@
     <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1367,17 +1459,14 @@
           <c:order val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Burndown!$A$2:$A$7</c:f>
+              <c:f>Burndown!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>m/d</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>42406</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42419</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>42422</c:v>
                 </c:pt>
               </c:numCache>
@@ -1385,17 +1474,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$B$2:$B$7</c:f>
+              <c:f>Burndown!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
@@ -1929,13 +2015,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>948267</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>160867</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>397934</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>25401</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2429,8 +2515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2629,86 +2715,176 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
       <c r="B12" t="s">
         <v>136</v>
       </c>
       <c r="C12" t="s">
         <v>91</v>
       </c>
+      <c r="D12" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2</v>
+      </c>
       <c r="B13" t="s">
         <v>137</v>
       </c>
       <c r="C13" t="s">
         <v>92</v>
       </c>
+      <c r="D13" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2</v>
+      </c>
       <c r="B14" t="s">
         <v>138</v>
       </c>
       <c r="C14" t="s">
         <v>94</v>
       </c>
+      <c r="D14" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2</v>
+      </c>
       <c r="B15" t="s">
         <v>139</v>
       </c>
       <c r="C15" t="s">
         <v>188</v>
       </c>
+      <c r="D15" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2</v>
+      </c>
       <c r="B16" t="s">
         <v>140</v>
       </c>
       <c r="C16" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D16" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2</v>
+      </c>
       <c r="B17" t="s">
         <v>141</v>
       </c>
       <c r="C17" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D17" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2</v>
+      </c>
       <c r="B18" t="s">
         <v>142</v>
       </c>
       <c r="C18" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D18" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2</v>
+      </c>
       <c r="B19" t="s">
         <v>143</v>
       </c>
       <c r="C19" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D19" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2</v>
+      </c>
       <c r="B20" t="s">
         <v>144</v>
       </c>
       <c r="C20" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D20" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2</v>
+      </c>
       <c r="B21" t="s">
         <v>145</v>
       </c>
       <c r="C21" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D21" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>146</v>
       </c>
@@ -2716,7 +2892,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>147</v>
       </c>
@@ -2724,7 +2900,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>148</v>
       </c>
@@ -2732,7 +2908,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>149</v>
       </c>
@@ -2740,7 +2916,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>150</v>
       </c>
@@ -2748,7 +2924,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>151</v>
       </c>
@@ -2756,7 +2932,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>152</v>
       </c>
@@ -2764,7 +2940,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>153</v>
       </c>
@@ -2772,7 +2948,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>154</v>
       </c>
@@ -2780,7 +2956,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>155</v>
       </c>
@@ -2788,7 +2964,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>156</v>
       </c>
@@ -3087,10 +3263,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3145,44 +3321,22 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>42419</v>
+        <v>42422</v>
       </c>
       <c r="B3">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C3">
-        <f>B2-B3</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>250</v>
+        <v>450</v>
       </c>
       <c r="E3">
-        <v>120</v>
+        <v>436</v>
       </c>
       <c r="F3" s="9">
-        <f>(D3-D2)/E3*60</f>
-        <v>125.00000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>42422</v>
-      </c>
-      <c r="B4">
-        <v>30</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>450</v>
-      </c>
-      <c r="E4">
-        <v>436</v>
-      </c>
-      <c r="F4" s="9">
-        <f>D4/E4 * 60</f>
+        <f>D3/E3 * 60</f>
         <v>61.926605504587151</v>
       </c>
     </row>
@@ -3198,8 +3352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:Q8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3466,10 +3620,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3616,6 +3770,9 @@
       <c r="C5" t="s">
         <v>217</v>
       </c>
+      <c r="D5" s="27" t="s">
+        <v>238</v>
+      </c>
       <c r="E5">
         <v>30</v>
       </c>
@@ -3679,6 +3836,9 @@
       <c r="C8" t="s">
         <v>217</v>
       </c>
+      <c r="D8" s="27" t="s">
+        <v>238</v>
+      </c>
       <c r="E8">
         <v>30</v>
       </c>
@@ -3757,8 +3917,8 @@
       <c r="P11" t="s">
         <v>273</v>
       </c>
-      <c r="Q11" s="20">
-        <v>42495</v>
+      <c r="Q11" s="21" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
@@ -3804,8 +3964,8 @@
       <c r="P14" t="s">
         <v>274</v>
       </c>
-      <c r="Q14" s="20">
-        <v>42495</v>
+      <c r="Q14" s="21" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
@@ -3818,6 +3978,9 @@
       <c r="C17" t="s">
         <v>230</v>
       </c>
+      <c r="D17" s="27" t="s">
+        <v>238</v>
+      </c>
       <c r="E17">
         <v>30</v>
       </c>
@@ -4040,10 +4203,41 @@
         <v>252</v>
       </c>
     </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H34">
-        <f>SUM(H2:H29)</f>
-        <v>436</v>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B31" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="27" t="s">
+        <v>303</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35" s="27" t="s">
+        <v>304</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36" s="27" t="s">
+        <v>305</v>
+      </c>
+      <c r="D36" s="27" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -4055,15 +4249,28 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView topLeftCell="G3" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.81640625" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" customWidth="1"/>
+    <col min="6" max="6" width="8.54296875" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" customWidth="1"/>
+    <col min="10" max="10" width="9.26953125" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" customWidth="1"/>
+    <col min="13" max="13" width="12.08984375" customWidth="1"/>
+    <col min="14" max="14" width="2.7265625" customWidth="1"/>
+    <col min="16" max="16" width="13.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -4077,7 +4284,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>16</v>
+        <v>301</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>17</v>
@@ -4090,11 +4297,231 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>20</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="N1" s="17"/>
+      <c r="O1" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="E2">
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="E8">
+        <v>30</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="E9">
+        <v>30</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="E10">
+        <v>40</v>
+      </c>
+      <c r="F10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="E11">
+        <v>40</v>
+      </c>
+      <c r="F11">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4176,10 +4603,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4188,7 +4615,7 @@
     <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>125</v>
       </c>
@@ -4199,117 +4626,117 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="26" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="26" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="26" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="26" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="26" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="26" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A11" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="26" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>136</v>
       </c>
@@ -4319,8 +4746,11 @@
       <c r="C12" s="12" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>137</v>
       </c>
@@ -4330,8 +4760,11 @@
       <c r="C13" s="12" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>138</v>
       </c>
@@ -4341,8 +4774,11 @@
       <c r="C14" s="12" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>139</v>
       </c>
@@ -4352,8 +4788,11 @@
       <c r="C15" s="12" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>140</v>
       </c>
@@ -4363,8 +4802,11 @@
       <c r="C16" s="12" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>141</v>
       </c>
@@ -4374,8 +4816,11 @@
       <c r="C17" s="12" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>142</v>
       </c>
@@ -4385,8 +4830,11 @@
       <c r="C18" s="12" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>143</v>
       </c>
@@ -4396,8 +4844,11 @@
       <c r="C19" s="12" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>144</v>
       </c>
@@ -4407,8 +4858,11 @@
       <c r="C20" s="12" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>145</v>
       </c>
@@ -4418,8 +4872,11 @@
       <c r="C21" s="12" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>146</v>
       </c>
@@ -4429,8 +4886,11 @@
       <c r="C22" s="12" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>147</v>
       </c>
@@ -4440,8 +4900,11 @@
       <c r="C23" s="12" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>148</v>
       </c>
@@ -4451,8 +4914,11 @@
       <c r="C24" s="12" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>149</v>
       </c>
@@ -4462,8 +4928,11 @@
       <c r="C25" s="12" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>150</v>
       </c>
@@ -4473,8 +4942,11 @@
       <c r="C26" s="12" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>151</v>
       </c>
@@ -4484,8 +4956,11 @@
       <c r="C27" s="12" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>152</v>
       </c>
@@ -4495,8 +4970,11 @@
       <c r="C28" s="12" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>153</v>
       </c>
@@ -4506,8 +4984,11 @@
       <c r="C29" s="12" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>154</v>
       </c>
@@ -4517,8 +4998,11 @@
       <c r="C30" s="12" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>155</v>
       </c>
@@ -4528,8 +5012,11 @@
       <c r="C31" s="12" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>156</v>
       </c>
@@ -4539,8 +5026,11 @@
       <c r="C32" s="12" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>157</v>
       </c>
@@ -4550,8 +5040,11 @@
       <c r="C33" s="12" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>158</v>
       </c>
@@ -4561,8 +5054,11 @@
       <c r="C34" s="12" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>159</v>
       </c>
@@ -4572,8 +5068,11 @@
       <c r="C35" s="12" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>160</v>
       </c>
@@ -4583,8 +5082,11 @@
       <c r="C36" s="12" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>161</v>
       </c>
@@ -4594,8 +5096,11 @@
       <c r="C37" s="12" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>162</v>
       </c>
@@ -4605,8 +5110,11 @@
       <c r="C38" s="12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>163</v>
       </c>
@@ -4616,8 +5124,11 @@
       <c r="C39" s="12" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>164</v>
       </c>
@@ -4627,8 +5138,11 @@
       <c r="C40" s="12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>165</v>
       </c>
@@ -4638,8 +5152,11 @@
       <c r="C41" s="12" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>166</v>
       </c>
@@ -4649,8 +5166,11 @@
       <c r="C42" s="12" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>167</v>
       </c>
@@ -4659,6 +5179,9 @@
       </c>
       <c r="C43" s="12" t="s">
         <v>78</v>
+      </c>
+      <c r="D43" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use cases 11 and 16
Completed use cases 11 and 16
</commit_message>
<xml_diff>
--- a/TeamDRAINReport.xlsx
+++ b/TeamDRAINReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16098\Desktop\SSW555_DRAIN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanqin/Desktop/SSW555_DRAIN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E0D10B-26B0-4FF8-BDA9-62AF6E196A00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6687B3-70E3-9243-A711-48A702216B00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19240" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -1324,7 +1324,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1395,7 +1395,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2376,15 +2376,15 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.453125" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" customWidth="1"/>
-    <col min="4" max="5" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>21</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>212</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>217</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>230</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>224</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>227</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>45</v>
       </c>
@@ -2515,19 +2515,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.08984375" customWidth="1"/>
-    <col min="3" max="3" width="28.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>35</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2748,7 +2748,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2850,7 +2850,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B22" t="s">
         <v>146</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B23" t="s">
         <v>147</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B24" t="s">
         <v>148</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B25" t="s">
         <v>149</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B26" t="s">
         <v>150</v>
       </c>
@@ -2924,7 +2924,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B27" t="s">
         <v>151</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
         <v>152</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B29" t="s">
         <v>153</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B30" t="s">
         <v>154</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B31" t="s">
         <v>155</v>
       </c>
@@ -2964,7 +2964,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
         <v>156</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B33" t="s">
         <v>157</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B34" t="s">
         <v>158</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B35" t="s">
         <v>159</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B36" t="s">
         <v>160</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B37" t="s">
         <v>161</v>
       </c>
@@ -3012,7 +3012,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B38" t="s">
         <v>162</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B39" t="s">
         <v>163</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B40" t="s">
         <v>164</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B41" t="s">
         <v>165</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B42" t="s">
         <v>166</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B43" t="s">
         <v>167</v>
       </c>
@@ -3075,47 +3075,47 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="7"/>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>179</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>180</v>
       </c>
@@ -3154,7 +3154,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>181</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
         <v>182</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>183</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>184</v>
       </c>
@@ -3269,17 +3269,17 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="2"/>
-    <col min="2" max="2" width="16.6328125" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="7.08984375" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>42406</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>42422</v>
       </c>
@@ -3356,27 +3356,27 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" customWidth="1"/>
-    <col min="6" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.453125" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.08984375" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.90625" style="17" customWidth="1"/>
-    <col min="15" max="15" width="10.08984375" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.453125" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.08984375" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.83203125" style="17" customWidth="1"/>
+    <col min="15" max="15" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -3470,7 +3470,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>168</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>169</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>170</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>130</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>171</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>172</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>173</v>
       </c>
@@ -3577,36 +3577,36 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" ht="28" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" ht="28" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" ht="28" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
         <v>47</v>
       </c>
@@ -3626,27 +3626,27 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.36328125" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6328125" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="2" customWidth="1"/>
-    <col min="15" max="15" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>126</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
       <c r="M3" s="17"/>
@@ -3751,7 +3751,7 @@
       <c r="P3" s="17"/>
       <c r="Q3" s="17"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
@@ -3760,7 +3760,7 @@
       <c r="P4" s="17"/>
       <c r="Q4" s="17"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="K6" s="17"/>
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
@@ -3817,7 +3817,7 @@
       <c r="P6" s="17"/>
       <c r="Q6" s="17"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
       <c r="M7" s="17"/>
@@ -3826,7 +3826,7 @@
       <c r="P7" s="17"/>
       <c r="Q7" s="17"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>129</v>
       </c>
@@ -3921,7 +3921,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>130</v>
       </c>
@@ -3968,7 +3968,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>131</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -4062,7 +4062,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>133</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>134</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>135</v>
       </c>
@@ -4203,12 +4203,12 @@
         <v>252</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B31" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="4" t="s">
         <v>300</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B34" s="27" t="s">
         <v>303</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B35" s="27" t="s">
         <v>304</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B36" s="27" t="s">
         <v>305</v>
       </c>
@@ -4251,26 +4251,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C11"/>
+    <sheetView tabSelected="1" zoomScale="227" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.6328125" customWidth="1"/>
-    <col min="2" max="2" width="24.81640625" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" customWidth="1"/>
-    <col min="6" max="6" width="8.54296875" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" customWidth="1"/>
-    <col min="10" max="10" width="9.26953125" customWidth="1"/>
-    <col min="12" max="12" width="15.453125" customWidth="1"/>
-    <col min="13" max="13" width="12.08984375" customWidth="1"/>
-    <col min="14" max="14" width="2.7265625" customWidth="1"/>
-    <col min="16" max="16" width="13.26953125" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" customWidth="1"/>
+    <col min="6" max="7" width="8.5" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15.5" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" customWidth="1"/>
+    <col min="14" max="14" width="2.6640625" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -4318,7 +4317,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -4337,8 +4336,11 @@
       <c r="F2">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -4358,7 +4360,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -4378,7 +4380,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>139</v>
       </c>
@@ -4398,7 +4400,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -4418,7 +4420,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -4437,8 +4439,11 @@
       <c r="F7">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>142</v>
       </c>
@@ -4457,8 +4462,11 @@
       <c r="F8">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>143</v>
       </c>
@@ -4477,8 +4485,11 @@
       <c r="F9">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>144</v>
       </c>
@@ -4498,7 +4509,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>145</v>
       </c>
@@ -4533,13 +4544,13 @@
       <selection activeCell="A2" sqref="A2:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="27.6328125" customWidth="1"/>
-    <col min="3" max="3" width="31.36328125" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -4568,31 +4579,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C2" s="12"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C3" s="12"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C4" s="12"/>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C5" s="12"/>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C6" s="12"/>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C9" s="12"/>
     </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C10" s="12"/>
     </row>
   </sheetData>
@@ -4605,17 +4616,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C37" sqref="C36:C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>125</v>
       </c>
@@ -4626,7 +4637,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="25" t="s">
         <v>126</v>
       </c>
@@ -4637,7 +4648,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" s="25" t="s">
         <v>127</v>
       </c>
@@ -4648,7 +4659,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="25" t="s">
         <v>128</v>
       </c>
@@ -4659,7 +4670,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" s="25" t="s">
         <v>129</v>
       </c>
@@ -4670,7 +4681,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" s="25" t="s">
         <v>130</v>
       </c>
@@ -4681,7 +4692,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" s="25" t="s">
         <v>131</v>
       </c>
@@ -4692,7 +4703,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" s="25" t="s">
         <v>132</v>
       </c>
@@ -4703,7 +4714,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" s="25" t="s">
         <v>133</v>
       </c>
@@ -4714,7 +4725,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" s="25" t="s">
         <v>134</v>
       </c>
@@ -4725,7 +4736,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" s="25" t="s">
         <v>135</v>
       </c>
@@ -4736,7 +4747,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>136</v>
       </c>
@@ -4750,7 +4761,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>137</v>
       </c>
@@ -4764,7 +4775,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>138</v>
       </c>
@@ -4778,7 +4789,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>139</v>
       </c>
@@ -4792,7 +4803,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>140</v>
       </c>
@@ -4806,7 +4817,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>141</v>
       </c>
@@ -4820,7 +4831,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>142</v>
       </c>
@@ -4834,7 +4845,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>143</v>
       </c>
@@ -4848,7 +4859,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>144</v>
       </c>
@@ -4862,7 +4873,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>145</v>
       </c>
@@ -4876,7 +4887,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>146</v>
       </c>
@@ -4890,7 +4901,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>147</v>
       </c>
@@ -4904,7 +4915,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>148</v>
       </c>
@@ -4918,7 +4929,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>149</v>
       </c>
@@ -4932,7 +4943,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>150</v>
       </c>
@@ -4946,7 +4957,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="136" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>151</v>
       </c>
@@ -4960,7 +4971,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>152</v>
       </c>
@@ -4974,7 +4985,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>153</v>
       </c>
@@ -4988,7 +4999,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>154</v>
       </c>
@@ -5002,7 +5013,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>155</v>
       </c>
@@ -5016,7 +5027,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>156</v>
       </c>
@@ -5030,7 +5041,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>157</v>
       </c>
@@ -5044,7 +5055,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>158</v>
       </c>
@@ -5058,7 +5069,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>159</v>
       </c>
@@ -5072,7 +5083,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>160</v>
       </c>
@@ -5086,7 +5097,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>161</v>
       </c>
@@ -5100,7 +5111,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>162</v>
       </c>
@@ -5114,7 +5125,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>163</v>
       </c>
@@ -5128,7 +5139,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>164</v>
       </c>
@@ -5142,7 +5153,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>165</v>
       </c>
@@ -5156,7 +5167,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>166</v>
       </c>
@@ -5170,7 +5181,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>167</v>
       </c>

</xml_diff>

<commit_message>
Updated Excel sheet and Integrated User Stories
</commit_message>
<xml_diff>
--- a/TeamDRAINReport.xlsx
+++ b/TeamDRAINReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanqin/Desktop/SSW555_DRAIN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6687B3-70E3-9243-A711-48A702216B00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54837CD-EC61-0F43-9B78-F9700BEB98C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19240" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="322">
   <si>
     <t>Find marriage date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1012,6 +1012,45 @@
   </si>
   <si>
     <t>Assigned</t>
+  </si>
+  <si>
+    <t>checkUS11</t>
+  </si>
+  <si>
+    <t>checkUS16</t>
+  </si>
+  <si>
+    <t>checkUS17</t>
+  </si>
+  <si>
+    <t>checkUS18</t>
+  </si>
+  <si>
+    <t>testUS11.py</t>
+  </si>
+  <si>
+    <t>testUS16.py</t>
+  </si>
+  <si>
+    <t>testUS17.py</t>
+  </si>
+  <si>
+    <t>testUS18.py</t>
+  </si>
+  <si>
+    <t>testUS11</t>
+  </si>
+  <si>
+    <t>testUS16</t>
+  </si>
+  <si>
+    <t>testUS17</t>
+  </si>
+  <si>
+    <t>testUS18</t>
+  </si>
+  <si>
+    <t>5-7</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1205,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1215,6 +1254,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1468,6 +1508,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>42422</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42436</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2515,8 +2558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2728,7 +2771,7 @@
         <v>227</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>308</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
@@ -2813,7 +2856,7 @@
         <v>227</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>308</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
@@ -2830,7 +2873,7 @@
         <v>224</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>308</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
@@ -2847,7 +2890,7 @@
         <v>224</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>308</v>
+        <v>253</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
@@ -3263,10 +3306,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3338,6 +3381,11 @@
       <c r="F3" s="9">
         <f>D3/E3 * 60</f>
         <v>61.926605504587151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="2">
+        <v>42436</v>
       </c>
     </row>
   </sheetData>
@@ -3623,7 +3671,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3637,7 +3685,7 @@
     <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
     <col min="12" max="12" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="2" customWidth="1"/>
@@ -4251,8 +4299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="227" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4263,6 +4311,7 @@
     <col min="5" max="5" width="9.1640625" customWidth="1"/>
     <col min="6" max="7" width="8.5" customWidth="1"/>
     <col min="10" max="10" width="9.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.5" customWidth="1"/>
     <col min="13" max="13" width="12.1640625" customWidth="1"/>
     <col min="14" max="14" width="2.6640625" customWidth="1"/>
@@ -4336,8 +4385,29 @@
       <c r="F2">
         <v>45</v>
       </c>
+      <c r="G2">
+        <v>96</v>
+      </c>
       <c r="H2">
         <v>54</v>
+      </c>
+      <c r="I2" s="20">
+        <v>42435</v>
+      </c>
+      <c r="K2" t="s">
+        <v>239</v>
+      </c>
+      <c r="L2" t="s">
+        <v>309</v>
+      </c>
+      <c r="O2" t="s">
+        <v>313</v>
+      </c>
+      <c r="P2" t="s">
+        <v>317</v>
+      </c>
+      <c r="Q2" s="23" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.15">
@@ -4439,8 +4509,29 @@
       <c r="F7">
         <v>60</v>
       </c>
+      <c r="G7">
+        <v>19</v>
+      </c>
       <c r="H7">
         <v>27</v>
+      </c>
+      <c r="I7" s="20">
+        <v>42435</v>
+      </c>
+      <c r="K7" t="s">
+        <v>239</v>
+      </c>
+      <c r="L7" t="s">
+        <v>310</v>
+      </c>
+      <c r="O7" t="s">
+        <v>314</v>
+      </c>
+      <c r="P7" t="s">
+        <v>318</v>
+      </c>
+      <c r="Q7" s="28" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.15">
@@ -4462,8 +4553,29 @@
       <c r="F8">
         <v>100</v>
       </c>
+      <c r="G8">
+        <v>30</v>
+      </c>
       <c r="H8">
         <v>75</v>
+      </c>
+      <c r="I8" s="20">
+        <v>42435</v>
+      </c>
+      <c r="K8" t="s">
+        <v>239</v>
+      </c>
+      <c r="L8" t="s">
+        <v>311</v>
+      </c>
+      <c r="O8" t="s">
+        <v>315</v>
+      </c>
+      <c r="P8" t="s">
+        <v>319</v>
+      </c>
+      <c r="Q8" s="28" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.15">
@@ -4485,8 +4597,29 @@
       <c r="F9">
         <v>100</v>
       </c>
+      <c r="G9">
+        <v>27</v>
+      </c>
       <c r="H9">
         <v>72</v>
+      </c>
+      <c r="I9" s="20">
+        <v>42435</v>
+      </c>
+      <c r="K9" t="s">
+        <v>239</v>
+      </c>
+      <c r="L9" t="s">
+        <v>312</v>
+      </c>
+      <c r="O9" t="s">
+        <v>316</v>
+      </c>
+      <c r="P9" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q9" s="28" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.15">
@@ -4971,7 +5104,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>152</v>
       </c>

</xml_diff>

<commit_message>
updated team report Backlog and Burndown
</commit_message>
<xml_diff>
--- a/TeamDRAINReport.xlsx
+++ b/TeamDRAINReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miahn\Documents\cs555\SSW555_DRAIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76A39C3-2A1D-4D77-88BA-4FEDE36A1AE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE77CF59-6DB8-414B-9C48-0537827AE902}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,9 @@
     <sheet name="sample sprint" sheetId="3" r:id="rId5"/>
     <sheet name="Sprint1" sheetId="4" r:id="rId6"/>
     <sheet name="Sprint2" sheetId="5" r:id="rId7"/>
-    <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
-    <sheet name="Stories" sheetId="11" r:id="rId9"/>
+    <sheet name="Sprint3" sheetId="14" r:id="rId8"/>
+    <sheet name="Sprint4" sheetId="6" r:id="rId9"/>
+    <sheet name="Stories" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="352">
   <si>
     <t>Find marriage date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1614,6 +1615,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2642,12 +2646,601 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A14" zoomScale="104" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C37" sqref="C36:C37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A11" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15" t="s">
+        <v>188</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" t="s">
+        <v>195</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D18" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>145</v>
+      </c>
+      <c r="B21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>146</v>
+      </c>
+      <c r="B22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>147</v>
+      </c>
+      <c r="B23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>149</v>
+      </c>
+      <c r="B25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B26" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>151</v>
+      </c>
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="D27" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>153</v>
+      </c>
+      <c r="B29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="D29" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>154</v>
+      </c>
+      <c r="B30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>155</v>
+      </c>
+      <c r="B31" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>156</v>
+      </c>
+      <c r="B32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>157</v>
+      </c>
+      <c r="B33" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>159</v>
+      </c>
+      <c r="B35" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>160</v>
+      </c>
+      <c r="B36" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>161</v>
+      </c>
+      <c r="B37" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>162</v>
+      </c>
+      <c r="B38" t="s">
+        <v>117</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>163</v>
+      </c>
+      <c r="B39" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>164</v>
+      </c>
+      <c r="B40" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>165</v>
+      </c>
+      <c r="B41" t="s">
+        <v>120</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>166</v>
+      </c>
+      <c r="B42" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>167</v>
+      </c>
+      <c r="B43" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" t="s">
+        <v>299</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="A16" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3292,8 +3885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3487,7 +4080,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3564,6 +4157,23 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>42436</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <f>349+450</f>
+        <v>799</v>
+      </c>
+      <c r="E4">
+        <v>633</v>
+      </c>
+      <c r="F4" s="9">
+        <f>(D4-D3)/E4 * 60</f>
+        <v>33.080568720379148</v>
       </c>
     </row>
   </sheetData>
@@ -3848,7 +4458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
@@ -4477,8 +5087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -5068,11 +5678,351 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDC2923-12C2-4914-B422-2854C29C5C4E}">
+  <dimension ref="A1:Q23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="N1" s="17"/>
+      <c r="O1" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2">
+        <v>40</v>
+      </c>
+      <c r="F2">
+        <v>60</v>
+      </c>
+      <c r="I2" s="20"/>
+      <c r="K2" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q2" s="23"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+      <c r="I3" s="20"/>
+      <c r="K3" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q3" s="28"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>40</v>
+      </c>
+      <c r="I4" s="20"/>
+      <c r="K4" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q4" s="28"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="E5">
+        <v>40</v>
+      </c>
+      <c r="F5">
+        <v>60</v>
+      </c>
+      <c r="I5" s="13"/>
+      <c r="K5" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q5" s="23"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+      <c r="F6">
+        <v>45</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="K6" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q6" s="28"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>60</v>
+      </c>
+      <c r="I7" s="20"/>
+      <c r="K7" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q7" s="28"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>45</v>
+      </c>
+      <c r="I8" s="20"/>
+      <c r="K8" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q8" s="28"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>45</v>
+      </c>
+      <c r="I9" s="20"/>
+      <c r="K9" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q9" s="28"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="E10">
+        <v>40</v>
+      </c>
+      <c r="F10">
+        <v>60</v>
+      </c>
+      <c r="I10" s="20"/>
+      <c r="K10" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q10" s="23"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="E11">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>40</v>
+      </c>
+      <c r="I11" s="20"/>
+      <c r="K11" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q11" s="28"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="27"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="27"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="27"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="27"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="27"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -5141,593 +6091,4 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D43"/>
-  <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="104" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C37" sqref="C36:C37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A10" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>136</v>
-      </c>
-      <c r="B12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>137</v>
-      </c>
-      <c r="B13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>138</v>
-      </c>
-      <c r="B14" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="D14" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>139</v>
-      </c>
-      <c r="B15" t="s">
-        <v>188</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>140</v>
-      </c>
-      <c r="B16" t="s">
-        <v>95</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B17" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>142</v>
-      </c>
-      <c r="B18" t="s">
-        <v>195</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D18" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>143</v>
-      </c>
-      <c r="B19" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>144</v>
-      </c>
-      <c r="B20" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>145</v>
-      </c>
-      <c r="B21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>146</v>
-      </c>
-      <c r="B22" t="s">
-        <v>100</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="D22" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>147</v>
-      </c>
-      <c r="B23" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="D23" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>148</v>
-      </c>
-      <c r="B24" t="s">
-        <v>104</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>149</v>
-      </c>
-      <c r="B25" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>150</v>
-      </c>
-      <c r="B26" t="s">
-        <v>106</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>151</v>
-      </c>
-      <c r="B27" t="s">
-        <v>107</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="D27" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>152</v>
-      </c>
-      <c r="B28" t="s">
-        <v>108</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>153</v>
-      </c>
-      <c r="B29" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="D29" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>154</v>
-      </c>
-      <c r="B30" t="s">
-        <v>110</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D30" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>155</v>
-      </c>
-      <c r="B31" t="s">
-        <v>111</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>156</v>
-      </c>
-      <c r="B32" t="s">
-        <v>112</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>157</v>
-      </c>
-      <c r="B33" t="s">
-        <v>113</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>158</v>
-      </c>
-      <c r="B34" t="s">
-        <v>114</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D34" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>159</v>
-      </c>
-      <c r="B35" t="s">
-        <v>124</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>160</v>
-      </c>
-      <c r="B36" t="s">
-        <v>115</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>161</v>
-      </c>
-      <c r="B37" t="s">
-        <v>116</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="D37" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>162</v>
-      </c>
-      <c r="B38" t="s">
-        <v>117</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D38" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>163</v>
-      </c>
-      <c r="B39" t="s">
-        <v>118</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D39" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>164</v>
-      </c>
-      <c r="B40" t="s">
-        <v>119</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="D40" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>165</v>
-      </c>
-      <c r="B41" t="s">
-        <v>120</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="D41" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>166</v>
-      </c>
-      <c r="B42" t="s">
-        <v>122</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D42" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>167</v>
-      </c>
-      <c r="B43" t="s">
-        <v>123</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D43" t="s">
-        <v>299</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
completed US29 and US30
</commit_message>
<xml_diff>
--- a/TeamDRAINReport.xlsx
+++ b/TeamDRAINReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miahn\Documents\cs555\SSW555_DRAIN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\SSW555_DRAIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE77CF59-6DB8-414B-9C48-0537827AE902}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5E1A3C-30D0-4C6E-9451-E558CA332A02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="362">
   <si>
     <t>Find marriage date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1140,6 +1142,36 @@
   </si>
   <si>
     <t>594-638</t>
+  </si>
+  <si>
+    <t>testUS29.py</t>
+  </si>
+  <si>
+    <t>testUS30.py</t>
+  </si>
+  <si>
+    <t>checkUS29()</t>
+  </si>
+  <si>
+    <t>checkUS30()</t>
+  </si>
+  <si>
+    <t>641-656</t>
+  </si>
+  <si>
+    <t>659-675</t>
+  </si>
+  <si>
+    <t>testUS29()</t>
+  </si>
+  <si>
+    <t>testUS30()</t>
+  </si>
+  <si>
+    <t>5-18</t>
+  </si>
+  <si>
+    <t>5-26</t>
   </si>
 </sst>
 </file>
@@ -1294,7 +1326,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1344,6 +1376,8 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3240,7 +3274,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:C33"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4079,7 +4113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -5087,7 +5121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="L1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -5681,11 +5715,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDC2923-12C2-4914-B422-2854C29C5C4E}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="8.7265625" customWidth="1"/>
+    <col min="9" max="9" width="12.1796875" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" customWidth="1"/>
+    <col min="12" max="12" width="17.54296875" customWidth="1"/>
+    <col min="15" max="15" width="11.453125" customWidth="1"/>
+    <col min="16" max="16" width="10.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
@@ -5758,7 +5800,7 @@
       <c r="K2" t="s">
         <v>239</v>
       </c>
-      <c r="Q2" s="23"/>
+      <c r="Q2" s="29"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -5783,7 +5825,7 @@
       <c r="K3" t="s">
         <v>239</v>
       </c>
-      <c r="Q3" s="28"/>
+      <c r="Q3" s="29"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -5808,7 +5850,7 @@
       <c r="K4" t="s">
         <v>239</v>
       </c>
-      <c r="Q4" s="28"/>
+      <c r="Q4" s="29"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -5833,7 +5875,7 @@
       <c r="K5" t="s">
         <v>239</v>
       </c>
-      <c r="Q5" s="23"/>
+      <c r="Q5" s="29"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -5858,7 +5900,7 @@
       <c r="K6" t="s">
         <v>239</v>
       </c>
-      <c r="Q6" s="28"/>
+      <c r="Q6" s="29"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -5883,7 +5925,7 @@
       <c r="K7" t="s">
         <v>239</v>
       </c>
-      <c r="Q7" s="28"/>
+      <c r="Q7" s="29"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -5904,11 +5946,33 @@
       <c r="F8">
         <v>45</v>
       </c>
-      <c r="I8" s="20"/>
+      <c r="G8">
+        <v>16</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8" s="20">
+        <v>42446</v>
+      </c>
       <c r="K8" t="s">
         <v>239</v>
       </c>
-      <c r="Q8" s="28"/>
+      <c r="L8" t="s">
+        <v>354</v>
+      </c>
+      <c r="M8" t="s">
+        <v>356</v>
+      </c>
+      <c r="O8" t="s">
+        <v>352</v>
+      </c>
+      <c r="P8" t="s">
+        <v>358</v>
+      </c>
+      <c r="Q8" s="30" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -5929,11 +5993,33 @@
       <c r="F9">
         <v>45</v>
       </c>
-      <c r="I9" s="20"/>
+      <c r="G9">
+        <v>16</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9" s="20">
+        <v>42446</v>
+      </c>
       <c r="K9" t="s">
         <v>239</v>
       </c>
-      <c r="Q9" s="28"/>
+      <c r="L9" t="s">
+        <v>355</v>
+      </c>
+      <c r="M9" t="s">
+        <v>357</v>
+      </c>
+      <c r="O9" t="s">
+        <v>353</v>
+      </c>
+      <c r="P9" t="s">
+        <v>359</v>
+      </c>
+      <c r="Q9" s="30" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -5958,7 +6044,7 @@
       <c r="K10" t="s">
         <v>239</v>
       </c>
-      <c r="Q10" s="23"/>
+      <c r="Q10" s="29"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -5983,7 +6069,7 @@
       <c r="K11" t="s">
         <v>239</v>
       </c>
-      <c r="Q11" s="28"/>
+      <c r="Q11" s="29"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
@@ -6014,6 +6100,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added comments and updated report for US21 and US23
</commit_message>
<xml_diff>
--- a/TeamDRAINReport.xlsx
+++ b/TeamDRAINReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\SSW555_DRAIN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16098\Desktop\SSW555_DRAIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5E1A3C-30D0-4C6E-9451-E558CA332A02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B58EA15-2804-4E3F-A79D-810EC69FA5A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="371">
   <si>
     <t>Find marriage date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1156,12 +1156,6 @@
     <t>checkUS30()</t>
   </si>
   <si>
-    <t>641-656</t>
-  </si>
-  <si>
-    <t>659-675</t>
-  </si>
-  <si>
     <t>testUS29()</t>
   </si>
   <si>
@@ -1172,6 +1166,39 @@
   </si>
   <si>
     <t>5-26</t>
+  </si>
+  <si>
+    <t>checkUS21()</t>
+  </si>
+  <si>
+    <t>checkUS23()</t>
+  </si>
+  <si>
+    <t>testUS21.py</t>
+  </si>
+  <si>
+    <t>testUS23.py</t>
+  </si>
+  <si>
+    <t>testUS21()</t>
+  </si>
+  <si>
+    <t>640-653</t>
+  </si>
+  <si>
+    <t>655-682</t>
+  </si>
+  <si>
+    <t>684-700</t>
+  </si>
+  <si>
+    <t>702-719</t>
+  </si>
+  <si>
+    <t>5-10</t>
+  </si>
+  <si>
+    <t>5-8</t>
   </si>
 </sst>
 </file>
@@ -3273,8 +3300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3656,7 +3683,7 @@
         <v>212</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>308</v>
+        <v>253</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -3690,7 +3717,7 @@
         <v>212</v>
       </c>
       <c r="E24" t="s">
-        <v>308</v>
+        <v>253</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -4113,7 +4140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -5715,12 +5742,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDC2923-12C2-4914-B422-2854C29C5C4E}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="24.36328125" customWidth="1"/>
     <col min="8" max="8" width="8.7265625" customWidth="1"/>
     <col min="9" max="9" width="12.1796875" customWidth="1"/>
     <col min="11" max="11" width="15.54296875" customWidth="1"/>
@@ -5796,11 +5824,33 @@
       <c r="F2">
         <v>60</v>
       </c>
-      <c r="I2" s="20"/>
+      <c r="G2">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+      <c r="I2" s="20">
+        <v>42456</v>
+      </c>
       <c r="K2" t="s">
         <v>239</v>
       </c>
-      <c r="Q2" s="29"/>
+      <c r="L2" t="s">
+        <v>360</v>
+      </c>
+      <c r="M2" t="s">
+        <v>365</v>
+      </c>
+      <c r="O2" t="s">
+        <v>362</v>
+      </c>
+      <c r="P2" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q2" s="23" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -5846,11 +5896,33 @@
       <c r="F4">
         <v>40</v>
       </c>
-      <c r="I4" s="20"/>
+      <c r="G4">
+        <v>27</v>
+      </c>
+      <c r="H4">
+        <v>40</v>
+      </c>
+      <c r="I4" s="20">
+        <v>42456</v>
+      </c>
       <c r="K4" t="s">
         <v>239</v>
       </c>
-      <c r="Q4" s="29"/>
+      <c r="L4" t="s">
+        <v>361</v>
+      </c>
+      <c r="M4" t="s">
+        <v>366</v>
+      </c>
+      <c r="O4" t="s">
+        <v>363</v>
+      </c>
+      <c r="P4" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q4" s="29" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -5962,16 +6034,16 @@
         <v>354</v>
       </c>
       <c r="M8" t="s">
-        <v>356</v>
+        <v>367</v>
       </c>
       <c r="O8" t="s">
         <v>352</v>
       </c>
       <c r="P8" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q8" s="30" t="s">
         <v>358</v>
-      </c>
-      <c r="Q8" s="30" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -6009,16 +6081,16 @@
         <v>355</v>
       </c>
       <c r="M9" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
       <c r="O9" t="s">
         <v>353</v>
       </c>
       <c r="P9" t="s">
+        <v>357</v>
+      </c>
+      <c r="Q9" s="30" t="s">
         <v>359</v>
-      </c>
-      <c r="Q9" s="30" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add U31 and U32 to Dana branch
</commit_message>
<xml_diff>
--- a/TeamDRAINReport.xlsx
+++ b/TeamDRAINReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\SSW555_DRAIN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dana/Stevens/cs555/SSW555_DRAIN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5E1A3C-30D0-4C6E-9451-E558CA332A02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC697E41-F6FF-1E45-9720-A5A28108FAF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1820" yWindow="460" windowWidth="33600" windowHeight="12580" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="372">
   <si>
     <t>Find marriage date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1172,6 +1172,36 @@
   </si>
   <si>
     <t>5-26</t>
+  </si>
+  <si>
+    <t>checkUS31()</t>
+  </si>
+  <si>
+    <t>678-695</t>
+  </si>
+  <si>
+    <t>testUS31.py</t>
+  </si>
+  <si>
+    <t>testUS31()</t>
+  </si>
+  <si>
+    <t>5-27</t>
+  </si>
+  <si>
+    <t>checkUS32()</t>
+  </si>
+  <si>
+    <t>697-711</t>
+  </si>
+  <si>
+    <t>testUS32.py</t>
+  </si>
+  <si>
+    <t>testUS32()</t>
+  </si>
+  <si>
+    <t>5-12</t>
   </si>
 </sst>
 </file>
@@ -1487,7 +1517,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1558,7 +1588,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2545,15 +2575,15 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.453125" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" customWidth="1"/>
-    <col min="4" max="5" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>21</v>
       </c>
@@ -2570,7 +2600,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>212</v>
       </c>
@@ -2587,7 +2617,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>217</v>
       </c>
@@ -2604,7 +2634,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>230</v>
       </c>
@@ -2621,7 +2651,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>224</v>
       </c>
@@ -2638,7 +2668,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>227</v>
       </c>
@@ -2655,7 +2685,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>45</v>
       </c>
@@ -2688,13 +2718,13 @@
       <selection activeCell="C37" sqref="C36:C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>125</v>
       </c>
@@ -2705,7 +2735,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" s="25" t="s">
         <v>126</v>
       </c>
@@ -2716,7 +2746,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" s="25" t="s">
         <v>127</v>
       </c>
@@ -2727,7 +2757,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="25" t="s">
         <v>128</v>
       </c>
@@ -2738,7 +2768,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" s="25" t="s">
         <v>129</v>
       </c>
@@ -2749,7 +2779,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A6" s="25" t="s">
         <v>130</v>
       </c>
@@ -2760,7 +2790,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" s="25" t="s">
         <v>131</v>
       </c>
@@ -2771,7 +2801,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" s="25" t="s">
         <v>132</v>
       </c>
@@ -2782,7 +2812,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" s="25" t="s">
         <v>133</v>
       </c>
@@ -2793,7 +2823,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" s="25" t="s">
         <v>134</v>
       </c>
@@ -2804,7 +2834,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A11" s="25" t="s">
         <v>135</v>
       </c>
@@ -2815,7 +2845,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>136</v>
       </c>
@@ -2829,7 +2859,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>137</v>
       </c>
@@ -2843,7 +2873,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>138</v>
       </c>
@@ -2857,7 +2887,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>139</v>
       </c>
@@ -2871,7 +2901,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>140</v>
       </c>
@@ -2885,7 +2915,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>141</v>
       </c>
@@ -2899,7 +2929,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>142</v>
       </c>
@@ -2913,7 +2943,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>143</v>
       </c>
@@ -2927,7 +2957,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>144</v>
       </c>
@@ -2941,7 +2971,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>145</v>
       </c>
@@ -2955,7 +2985,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>146</v>
       </c>
@@ -2969,7 +2999,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>147</v>
       </c>
@@ -2983,7 +3013,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>148</v>
       </c>
@@ -2997,7 +3027,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>149</v>
       </c>
@@ -3011,7 +3041,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>150</v>
       </c>
@@ -3025,7 +3055,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="136" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>151</v>
       </c>
@@ -3039,7 +3069,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>152</v>
       </c>
@@ -3053,7 +3083,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>153</v>
       </c>
@@ -3067,7 +3097,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>154</v>
       </c>
@@ -3081,7 +3111,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>155</v>
       </c>
@@ -3095,7 +3125,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>156</v>
       </c>
@@ -3109,7 +3139,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>157</v>
       </c>
@@ -3123,7 +3153,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>158</v>
       </c>
@@ -3137,7 +3167,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>159</v>
       </c>
@@ -3151,7 +3181,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>160</v>
       </c>
@@ -3165,7 +3195,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>161</v>
       </c>
@@ -3179,7 +3209,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>162</v>
       </c>
@@ -3193,7 +3223,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>163</v>
       </c>
@@ -3207,7 +3237,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>164</v>
       </c>
@@ -3221,7 +3251,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>165</v>
       </c>
@@ -3235,7 +3265,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>166</v>
       </c>
@@ -3249,7 +3279,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>167</v>
       </c>
@@ -3277,15 +3307,15 @@
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="3" max="3" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>35</v>
       </c>
@@ -3302,7 +3332,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3319,7 +3349,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3336,7 +3366,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3353,7 +3383,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3370,7 +3400,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3387,7 +3417,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3404,7 +3434,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3421,7 +3451,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1</v>
       </c>
@@ -3438,7 +3468,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3455,7 +3485,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3472,7 +3502,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2</v>
       </c>
@@ -3489,7 +3519,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2</v>
       </c>
@@ -3506,7 +3536,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2</v>
       </c>
@@ -3523,7 +3553,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3540,7 +3570,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2</v>
       </c>
@@ -3557,7 +3587,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2</v>
       </c>
@@ -3574,7 +3604,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3591,7 +3621,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3608,7 +3638,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2</v>
       </c>
@@ -3625,7 +3655,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2</v>
       </c>
@@ -3642,7 +3672,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>3</v>
       </c>
@@ -3659,7 +3689,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>3</v>
       </c>
@@ -3676,7 +3706,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>3</v>
       </c>
@@ -3693,7 +3723,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>3</v>
       </c>
@@ -3710,7 +3740,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>3</v>
       </c>
@@ -3727,7 +3757,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B27" t="s">
         <v>151</v>
       </c>
@@ -3735,7 +3765,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
         <v>152</v>
       </c>
@@ -3743,7 +3773,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3760,7 +3790,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>3</v>
       </c>
@@ -3777,7 +3807,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>3</v>
       </c>
@@ -3794,7 +3824,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>3</v>
       </c>
@@ -3811,7 +3841,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>3</v>
       </c>
@@ -3828,7 +3858,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B34" t="s">
         <v>158</v>
       </c>
@@ -3836,7 +3866,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B35" t="s">
         <v>159</v>
       </c>
@@ -3844,7 +3874,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B36" t="s">
         <v>160</v>
       </c>
@@ -3852,7 +3882,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B37" t="s">
         <v>161</v>
       </c>
@@ -3860,7 +3890,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B38" t="s">
         <v>162</v>
       </c>
@@ -3868,7 +3898,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B39" t="s">
         <v>163</v>
       </c>
@@ -3876,7 +3906,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B40" t="s">
         <v>164</v>
       </c>
@@ -3884,7 +3914,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B41" t="s">
         <v>165</v>
       </c>
@@ -3892,7 +3922,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B42" t="s">
         <v>166</v>
       </c>
@@ -3900,7 +3930,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B43" t="s">
         <v>167</v>
       </c>
@@ -3923,47 +3953,47 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="7"/>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>179</v>
       </c>
@@ -3986,7 +4016,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>180</v>
       </c>
@@ -4002,7 +4032,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>181</v>
       </c>
@@ -4027,7 +4057,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
         <v>182</v>
       </c>
@@ -4052,7 +4082,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>183</v>
       </c>
@@ -4077,7 +4107,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>184</v>
       </c>
@@ -4113,21 +4143,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="2"/>
-    <col min="2" max="2" width="16.6328125" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="7.1796875" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -4147,7 +4177,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>42406</v>
       </c>
@@ -4167,7 +4197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>42422</v>
       </c>
@@ -4188,7 +4218,7 @@
         <v>61.926605504587151</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>42436</v>
       </c>
@@ -4226,27 +4256,27 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.453125" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.81640625" style="17" customWidth="1"/>
-    <col min="15" max="15" width="10.1796875" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.453125" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.83203125" style="17" customWidth="1"/>
+    <col min="15" max="15" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -4293,7 +4323,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -4340,7 +4370,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>168</v>
       </c>
@@ -4351,7 +4381,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>169</v>
       </c>
@@ -4362,7 +4392,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>170</v>
       </c>
@@ -4373,7 +4403,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>130</v>
       </c>
@@ -4411,7 +4441,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>171</v>
       </c>
@@ -4425,7 +4455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>172</v>
       </c>
@@ -4436,7 +4466,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>173</v>
       </c>
@@ -4447,36 +4477,36 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B15" s="5"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" ht="28" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" ht="28" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" ht="14" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" ht="28" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
         <v>47</v>
       </c>
@@ -4496,27 +4526,27 @@
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.36328125" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6328125" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.36328125" customWidth="1"/>
-    <col min="12" max="12" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="2" customWidth="1"/>
-    <col min="15" max="15" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -4564,7 +4594,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>126</v>
       </c>
@@ -4612,7 +4642,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
       <c r="M3" s="17"/>
@@ -4621,7 +4651,7 @@
       <c r="P3" s="17"/>
       <c r="Q3" s="17"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
@@ -4630,7 +4660,7 @@
       <c r="P4" s="17"/>
       <c r="Q4" s="17"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -4678,7 +4708,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="K6" s="17"/>
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
@@ -4687,7 +4717,7 @@
       <c r="P6" s="17"/>
       <c r="Q6" s="17"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
       <c r="M7" s="17"/>
@@ -4696,7 +4726,7 @@
       <c r="P7" s="17"/>
       <c r="Q7" s="17"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -4744,7 +4774,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>129</v>
       </c>
@@ -4791,7 +4821,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>130</v>
       </c>
@@ -4838,7 +4868,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>131</v>
       </c>
@@ -4885,7 +4915,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -4932,7 +4962,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>133</v>
       </c>
@@ -4979,7 +5009,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>134</v>
       </c>
@@ -5026,7 +5056,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>135</v>
       </c>
@@ -5073,12 +5103,12 @@
         <v>252</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B31" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="4" t="s">
         <v>300</v>
       </c>
@@ -5086,7 +5116,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B34" s="27" t="s">
         <v>303</v>
       </c>
@@ -5094,7 +5124,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B35" s="27" t="s">
         <v>304</v>
       </c>
@@ -5102,7 +5132,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B36" s="27" t="s">
         <v>305</v>
       </c>
@@ -5125,22 +5155,22 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.6328125" customWidth="1"/>
-    <col min="2" max="2" width="24.81640625" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" customWidth="1"/>
-    <col min="6" max="7" width="8.453125" customWidth="1"/>
-    <col min="10" max="10" width="9.36328125" customWidth="1"/>
-    <col min="11" max="11" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.453125" customWidth="1"/>
-    <col min="13" max="13" width="12.1796875" customWidth="1"/>
-    <col min="14" max="14" width="2.6328125" customWidth="1"/>
-    <col min="16" max="16" width="13.36328125" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" customWidth="1"/>
+    <col min="6" max="7" width="8.5" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" customWidth="1"/>
+    <col min="14" max="14" width="2.6640625" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -5188,7 +5218,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -5235,7 +5265,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -5282,7 +5312,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -5329,7 +5359,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>139</v>
       </c>
@@ -5377,7 +5407,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -5424,7 +5454,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -5471,7 +5501,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>142</v>
       </c>
@@ -5518,7 +5548,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>143</v>
       </c>
@@ -5565,7 +5595,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>144</v>
       </c>
@@ -5612,7 +5642,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>145</v>
       </c>
@@ -5659,47 +5689,47 @@
         <v>321</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A16" s="27" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="27" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="27" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" s="27" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" s="27" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" s="27" t="s">
         <v>307</v>
       </c>
@@ -5715,21 +5745,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDC2923-12C2-4914-B422-2854C29C5C4E}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:Q13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="8" max="8" width="8.7265625" customWidth="1"/>
-    <col min="9" max="9" width="12.1796875" customWidth="1"/>
-    <col min="11" max="11" width="15.54296875" customWidth="1"/>
-    <col min="12" max="12" width="17.54296875" customWidth="1"/>
-    <col min="15" max="15" width="11.453125" customWidth="1"/>
-    <col min="16" max="16" width="10.26953125" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" customWidth="1"/>
+    <col min="11" max="11" width="15.5" customWidth="1"/>
+    <col min="12" max="12" width="17.5" customWidth="1"/>
+    <col min="15" max="15" width="11.5" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -5777,7 +5807,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>146</v>
       </c>
@@ -5802,7 +5832,7 @@
       </c>
       <c r="Q2" s="29"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>147</v>
       </c>
@@ -5827,7 +5857,7 @@
       </c>
       <c r="Q3" s="29"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>148</v>
       </c>
@@ -5852,7 +5882,7 @@
       </c>
       <c r="Q4" s="29"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>149</v>
       </c>
@@ -5877,7 +5907,7 @@
       </c>
       <c r="Q5" s="29"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>150</v>
       </c>
@@ -5902,7 +5932,7 @@
       </c>
       <c r="Q6" s="29"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>153</v>
       </c>
@@ -5927,7 +5957,7 @@
       </c>
       <c r="Q7" s="29"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>154</v>
       </c>
@@ -5974,7 +6004,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>155</v>
       </c>
@@ -6021,7 +6051,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>156</v>
       </c>
@@ -6046,7 +6076,7 @@
       </c>
       <c r="Q10" s="29"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>157</v>
       </c>
@@ -6071,31 +6101,122 @@
       </c>
       <c r="Q11" s="29"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="E12">
+        <v>40</v>
+      </c>
+      <c r="F12">
+        <v>60</v>
+      </c>
+      <c r="G12">
+        <v>17</v>
+      </c>
+      <c r="H12">
+        <v>15</v>
+      </c>
+      <c r="I12" s="20">
+        <v>42456</v>
+      </c>
+      <c r="K12" t="s">
+        <v>239</v>
+      </c>
+      <c r="L12" t="s">
+        <v>362</v>
+      </c>
+      <c r="M12" t="s">
+        <v>363</v>
+      </c>
+      <c r="O12" t="s">
+        <v>364</v>
+      </c>
+      <c r="P12" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q12" s="30" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
+      <c r="F13">
+        <v>40</v>
+      </c>
+      <c r="G13">
+        <v>14</v>
+      </c>
+      <c r="H13">
+        <v>45</v>
+      </c>
+      <c r="I13" s="20">
+        <v>42456</v>
+      </c>
+      <c r="K13" t="s">
+        <v>239</v>
+      </c>
+      <c r="L13" t="s">
+        <v>367</v>
+      </c>
+      <c r="M13" t="s">
+        <v>368</v>
+      </c>
+      <c r="O13" t="s">
+        <v>369</v>
+      </c>
+      <c r="P13" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q13" s="30" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A16" s="27"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="27"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" s="27"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" s="27"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" s="27"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" s="27"/>
     </row>
   </sheetData>
@@ -6112,13 +6233,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="27.6328125" customWidth="1"/>
-    <col min="3" max="3" width="31.36328125" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -6147,31 +6268,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C2" s="12"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C3" s="12"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C4" s="12"/>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C5" s="12"/>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C6" s="12"/>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C9" s="12"/>
     </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="C10" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished user stories 25 and 28
</commit_message>
<xml_diff>
--- a/TeamDRAINReport.xlsx
+++ b/TeamDRAINReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dana/Stevens/cs555/SSW555_DRAIN/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanqin/Desktop/SSW555_DRAIN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC697E41-F6FF-1E45-9720-A5A28108FAF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6622A211-13BF-3747-8DC6-49B71AABDCD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="460" windowWidth="33600" windowHeight="12580" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19240" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="380">
   <si>
     <t>Find marriage date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1202,6 +1202,30 @@
   </si>
   <si>
     <t>5-12</t>
+  </si>
+  <si>
+    <t>checkUS25()</t>
+  </si>
+  <si>
+    <t>testUS25.py</t>
+  </si>
+  <si>
+    <t>testUS25()</t>
+  </si>
+  <si>
+    <t>5-8</t>
+  </si>
+  <si>
+    <t>checkUS28()</t>
+  </si>
+  <si>
+    <t>testUS28.py</t>
+  </si>
+  <si>
+    <t>testUS28()</t>
+  </si>
+  <si>
+    <t>5-22</t>
   </si>
 </sst>
 </file>
@@ -5746,11 +5770,13 @@
   <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:Q13"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
     <col min="8" max="8" width="8.6640625" customWidth="1"/>
     <col min="9" max="9" width="12.1640625" customWidth="1"/>
     <col min="11" max="11" width="15.5" customWidth="1"/>
@@ -5901,7 +5927,7 @@
       <c r="F5">
         <v>60</v>
       </c>
-      <c r="I5" s="13"/>
+      <c r="I5" s="20"/>
       <c r="K5" t="s">
         <v>239</v>
       </c>
@@ -5926,11 +5952,30 @@
       <c r="F6">
         <v>45</v>
       </c>
-      <c r="I6" s="13"/>
+      <c r="G6">
+        <v>36</v>
+      </c>
+      <c r="H6">
+        <v>36</v>
+      </c>
+      <c r="I6" s="20">
+        <v>42457</v>
+      </c>
       <c r="K6" t="s">
         <v>239</v>
       </c>
-      <c r="Q6" s="29"/>
+      <c r="L6" t="s">
+        <v>372</v>
+      </c>
+      <c r="O6" t="s">
+        <v>373</v>
+      </c>
+      <c r="P6" t="s">
+        <v>374</v>
+      </c>
+      <c r="Q6" s="23" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
@@ -5951,11 +5996,30 @@
       <c r="F7">
         <v>60</v>
       </c>
-      <c r="I7" s="20"/>
+      <c r="G7">
+        <v>31</v>
+      </c>
+      <c r="H7">
+        <v>58</v>
+      </c>
+      <c r="I7" s="20">
+        <v>42457</v>
+      </c>
       <c r="K7" t="s">
         <v>239</v>
       </c>
-      <c r="Q7" s="29"/>
+      <c r="L7" t="s">
+        <v>376</v>
+      </c>
+      <c r="O7" t="s">
+        <v>377</v>
+      </c>
+      <c r="P7" t="s">
+        <v>378</v>
+      </c>
+      <c r="Q7" s="29" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" t="s">

</xml_diff>

<commit_message>
Completed US36 and US37 and Updated Sprint
</commit_message>
<xml_diff>
--- a/TeamDRAINReport.xlsx
+++ b/TeamDRAINReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\SSW555_DRAIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03EFAEA-FFBD-4EDB-9A55-56AF05B7C8E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE532CAD-D1D5-4B19-8A1F-F5B6ECDE1462}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="413">
   <si>
     <t>Find marriage date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1307,6 +1307,24 @@
   </si>
   <si>
     <t>Merge Conflicts</t>
+  </si>
+  <si>
+    <t>checkUS36()</t>
+  </si>
+  <si>
+    <t>testUS36()</t>
+  </si>
+  <si>
+    <t>testUS37()</t>
+  </si>
+  <si>
+    <t>checkUS37()</t>
+  </si>
+  <si>
+    <t>testUS36().py</t>
+  </si>
+  <si>
+    <t>testUS37().py</t>
   </si>
 </sst>
 </file>
@@ -5972,8 +5990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDC2923-12C2-4914-B422-2854C29C5C4E}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -6569,19 +6587,25 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="27.6328125" customWidth="1"/>
-    <col min="3" max="3" width="31.36328125" customWidth="1"/>
+    <col min="3" max="3" width="14.90625" customWidth="1"/>
+    <col min="12" max="12" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -6609,8 +6633,27 @@
       <c r="I1" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L1" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="O1" s="17"/>
+      <c r="P1" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>151</v>
       </c>
@@ -6629,8 +6672,11 @@
       <c r="F2">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>152</v>
       </c>
@@ -6649,8 +6695,11 @@
       <c r="F3">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>159</v>
       </c>
@@ -6669,8 +6718,11 @@
       <c r="F4">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>160</v>
       </c>
@@ -6689,8 +6741,11 @@
       <c r="F5">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>161</v>
       </c>
@@ -6701,7 +6756,7 @@
         <v>224</v>
       </c>
       <c r="D6" t="s">
-        <v>308</v>
+        <v>253</v>
       </c>
       <c r="E6">
         <v>20</v>
@@ -6709,8 +6764,32 @@
       <c r="F6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>19</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6" s="20">
+        <v>42469</v>
+      </c>
+      <c r="L6" t="s">
+        <v>239</v>
+      </c>
+      <c r="M6" t="s">
+        <v>407</v>
+      </c>
+      <c r="P6" t="s">
+        <v>411</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>408</v>
+      </c>
+      <c r="R6" s="23" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>162</v>
       </c>
@@ -6721,7 +6800,7 @@
         <v>224</v>
       </c>
       <c r="D7" t="s">
-        <v>308</v>
+        <v>253</v>
       </c>
       <c r="E7">
         <v>20</v>
@@ -6729,8 +6808,32 @@
       <c r="F7">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>30</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
+      </c>
+      <c r="I7" s="20">
+        <v>42469</v>
+      </c>
+      <c r="L7" t="s">
+        <v>239</v>
+      </c>
+      <c r="M7" t="s">
+        <v>410</v>
+      </c>
+      <c r="P7" t="s">
+        <v>412</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>409</v>
+      </c>
+      <c r="R7" s="28" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>163</v>
       </c>
@@ -6749,8 +6852,11 @@
       <c r="F8">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>164</v>
       </c>
@@ -6769,8 +6875,11 @@
       <c r="F9">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>165</v>
       </c>
@@ -6789,8 +6898,11 @@
       <c r="F10">
         <v>90</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L10" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>167</v>
       </c>
@@ -6808,6 +6920,9 @@
       </c>
       <c r="F11">
         <v>20</v>
+      </c>
+      <c r="L11" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed user stories 38 and 39
</commit_message>
<xml_diff>
--- a/TeamDRAINReport.xlsx
+++ b/TeamDRAINReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dana/Stevens/cs555/SSW555_DRAIN/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanqin/Desktop/SSW555_DRAIN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3CE174-DB16-D042-A94C-65C63EEB1891}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15C8BF8-1CB5-3C45-AFC0-E7F9EE50464B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="460" windowWidth="23260" windowHeight="7200" tabRatio="500" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19240" tabRatio="500" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="430">
   <si>
     <t>Find marriage date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1321,24 +1321,12 @@
     <t>checkUS37()</t>
   </si>
   <si>
-    <t>testUS36().py</t>
-  </si>
-  <si>
-    <t>testUS37().py</t>
-  </si>
-  <si>
     <t>checkUS34()</t>
   </si>
   <si>
     <t>checkUS35()</t>
   </si>
   <si>
-    <t>testUS34().py</t>
-  </si>
-  <si>
-    <t>testUS35().py</t>
-  </si>
-  <si>
     <t>testUS34()</t>
   </si>
   <si>
@@ -1358,6 +1346,36 @@
   </si>
   <si>
     <t>931-975</t>
+  </si>
+  <si>
+    <t>checkUS38()</t>
+  </si>
+  <si>
+    <t>checkUS39()</t>
+  </si>
+  <si>
+    <t>testUS38.py</t>
+  </si>
+  <si>
+    <t>testUS37.py</t>
+  </si>
+  <si>
+    <t>testUS36.py</t>
+  </si>
+  <si>
+    <t>testUS35.py</t>
+  </si>
+  <si>
+    <t>testUS34.py</t>
+  </si>
+  <si>
+    <t>testUS39.py</t>
+  </si>
+  <si>
+    <t>testUS38()</t>
+  </si>
+  <si>
+    <t>testUS39()</t>
   </si>
 </sst>
 </file>
@@ -2877,8 +2895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="104" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C37" sqref="C36:C37"/>
+    <sheetView topLeftCell="A27" zoomScale="104" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6622,8 +6640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6764,19 +6782,19 @@
         <v>239</v>
       </c>
       <c r="M4" t="s">
+        <v>411</v>
+      </c>
+      <c r="N4" t="s">
+        <v>416</v>
+      </c>
+      <c r="P4" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q4" t="s">
         <v>413</v>
       </c>
-      <c r="N4" t="s">
-        <v>420</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="R4" s="23" t="s">
         <v>415</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>417</v>
-      </c>
-      <c r="R4" s="23" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.15">
@@ -6811,16 +6829,16 @@
         <v>239</v>
       </c>
       <c r="M5" t="s">
+        <v>412</v>
+      </c>
+      <c r="N5" t="s">
+        <v>417</v>
+      </c>
+      <c r="P5" t="s">
+        <v>425</v>
+      </c>
+      <c r="Q5" t="s">
         <v>414</v>
-      </c>
-      <c r="N5" t="s">
-        <v>421</v>
-      </c>
-      <c r="P5" t="s">
-        <v>416</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>418</v>
       </c>
       <c r="R5" s="23" t="s">
         <v>399</v>
@@ -6861,10 +6879,10 @@
         <v>407</v>
       </c>
       <c r="N6" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="P6" t="s">
-        <v>411</v>
+        <v>424</v>
       </c>
       <c r="Q6" t="s">
         <v>408</v>
@@ -6908,10 +6926,10 @@
         <v>410</v>
       </c>
       <c r="N7" t="s">
+        <v>419</v>
+      </c>
+      <c r="P7" t="s">
         <v>423</v>
-      </c>
-      <c r="P7" t="s">
-        <v>412</v>
       </c>
       <c r="Q7" t="s">
         <v>409</v>
@@ -6939,8 +6957,29 @@
       <c r="F8">
         <v>30</v>
       </c>
+      <c r="G8">
+        <v>24</v>
+      </c>
+      <c r="H8">
+        <v>36</v>
+      </c>
+      <c r="I8" s="20">
+        <v>42471</v>
+      </c>
       <c r="L8" t="s">
         <v>239</v>
+      </c>
+      <c r="M8" t="s">
+        <v>420</v>
+      </c>
+      <c r="P8" t="s">
+        <v>422</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>428</v>
+      </c>
+      <c r="R8" s="23" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.15">
@@ -6962,8 +7001,29 @@
       <c r="F9">
         <v>45</v>
       </c>
+      <c r="G9">
+        <v>27</v>
+      </c>
+      <c r="H9">
+        <v>22</v>
+      </c>
+      <c r="I9" s="20">
+        <v>42471</v>
+      </c>
       <c r="L9" t="s">
         <v>239</v>
+      </c>
+      <c r="M9" t="s">
+        <v>421</v>
+      </c>
+      <c r="P9" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>429</v>
+      </c>
+      <c r="R9" s="23" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Updated sprint report backlog
</commit_message>
<xml_diff>
--- a/TeamDRAINReport.xlsx
+++ b/TeamDRAINReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miahn\Documents\cs555\SSW555_DRAIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE3E2A4-7E28-4C55-8757-E1C6EA3B0CF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1977D28F-1A64-4139-8972-BEB993494318}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -3565,8 +3565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -4049,8 +4049,8 @@
       <c r="D28" t="s">
         <v>230</v>
       </c>
-      <c r="E28" t="s">
-        <v>308</v>
+      <c r="E28" s="27" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -4168,8 +4168,8 @@
       <c r="D35" t="s">
         <v>217</v>
       </c>
-      <c r="E35" t="s">
-        <v>308</v>
+      <c r="E35" s="27" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -4185,8 +4185,8 @@
       <c r="D36" t="s">
         <v>217</v>
       </c>
-      <c r="E36" t="s">
-        <v>308</v>
+      <c r="E36" s="27" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -4202,8 +4202,8 @@
       <c r="D37" t="s">
         <v>224</v>
       </c>
-      <c r="E37" t="s">
-        <v>308</v>
+      <c r="E37" s="27" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -4219,8 +4219,8 @@
       <c r="D38" t="s">
         <v>224</v>
       </c>
-      <c r="E38" t="s">
-        <v>308</v>
+      <c r="E38" s="27" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -4236,8 +4236,8 @@
       <c r="D39" t="s">
         <v>227</v>
       </c>
-      <c r="E39" t="s">
-        <v>308</v>
+      <c r="E39" s="27" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -4253,8 +4253,8 @@
       <c r="D40" t="s">
         <v>227</v>
       </c>
-      <c r="E40" t="s">
-        <v>308</v>
+      <c r="E40" s="27" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -4495,7 +4495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -4650,7 +4650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -4920,7 +4920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
@@ -6742,7 +6742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changed Assigned to Completed where needed
</commit_message>
<xml_diff>
--- a/TeamDRAINReport.xlsx
+++ b/TeamDRAINReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miahn\Documents\cs555\SSW555_DRAIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1977D28F-1A64-4139-8972-BEB993494318}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241369CA-1BBF-4B0A-B40B-CC2221CFC483}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="454">
   <si>
     <t>Find marriage date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1010,9 +1010,6 @@
   </si>
   <si>
     <t>Not double checking code</t>
-  </si>
-  <si>
-    <t>Assigned</t>
   </si>
   <si>
     <t>checkUS11</t>
@@ -3565,7 +3562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
@@ -4920,7 +4917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
@@ -5549,7 +5546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:B23"/>
     </sheetView>
   </sheetViews>
@@ -5648,19 +5645,19 @@
         <v>239</v>
       </c>
       <c r="L2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="O2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="P2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Q2" s="23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -5695,19 +5692,19 @@
         <v>239</v>
       </c>
       <c r="L3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="M3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="O3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q3" s="28" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -5742,19 +5739,19 @@
         <v>239</v>
       </c>
       <c r="L4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="M4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="O4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="P4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q4" s="28" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -5790,19 +5787,19 @@
         <v>239</v>
       </c>
       <c r="L5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="M5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="O5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Q5" s="23" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -5837,19 +5834,19 @@
         <v>239</v>
       </c>
       <c r="L6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="M6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="O6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="P6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="Q6" s="28" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -5884,19 +5881,19 @@
         <v>239</v>
       </c>
       <c r="L7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="O7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="P7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q7" s="28" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -5931,19 +5928,19 @@
         <v>239</v>
       </c>
       <c r="L8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="O8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="P8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="Q8" s="28" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -5978,19 +5975,19 @@
         <v>239</v>
       </c>
       <c r="L9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="M9" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="O9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="P9" t="s">
+        <v>319</v>
+      </c>
+      <c r="Q9" s="28" t="s">
         <v>320</v>
-      </c>
-      <c r="Q9" s="28" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -6025,19 +6022,19 @@
         <v>239</v>
       </c>
       <c r="L10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="M10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="O10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="P10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Q10" s="23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -6072,19 +6069,19 @@
         <v>239</v>
       </c>
       <c r="L11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="M11" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="O11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="P11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Q11" s="28" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -6239,19 +6236,19 @@
         <v>239</v>
       </c>
       <c r="L2" t="s">
+        <v>393</v>
+      </c>
+      <c r="M2" t="s">
+        <v>390</v>
+      </c>
+      <c r="O2" t="s">
         <v>394</v>
       </c>
-      <c r="M2" t="s">
-        <v>391</v>
-      </c>
-      <c r="O2" t="s">
-        <v>395</v>
-      </c>
       <c r="P2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="Q2" s="21" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -6286,19 +6283,19 @@
         <v>239</v>
       </c>
       <c r="L3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="O3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="P3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="Q3" s="31" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -6333,19 +6330,19 @@
         <v>239</v>
       </c>
       <c r="L4" t="s">
+        <v>375</v>
+      </c>
+      <c r="M4" t="s">
+        <v>382</v>
+      </c>
+      <c r="O4" t="s">
         <v>376</v>
       </c>
-      <c r="M4" t="s">
-        <v>383</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>377</v>
       </c>
-      <c r="P4" t="s">
-        <v>378</v>
-      </c>
       <c r="Q4" s="29" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -6380,19 +6377,19 @@
         <v>239</v>
       </c>
       <c r="L5" t="s">
+        <v>367</v>
+      </c>
+      <c r="M5" t="s">
+        <v>383</v>
+      </c>
+      <c r="O5" t="s">
         <v>368</v>
       </c>
-      <c r="M5" t="s">
-        <v>384</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>369</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" s="23" t="s">
         <v>370</v>
-      </c>
-      <c r="Q5" s="23" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -6427,19 +6424,19 @@
         <v>239</v>
       </c>
       <c r="L6" t="s">
+        <v>371</v>
+      </c>
+      <c r="M6" t="s">
+        <v>384</v>
+      </c>
+      <c r="O6" t="s">
         <v>372</v>
       </c>
-      <c r="M6" t="s">
-        <v>385</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>373</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" s="29" t="s">
         <v>374</v>
-      </c>
-      <c r="Q6" s="29" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -6474,19 +6471,19 @@
         <v>239</v>
       </c>
       <c r="L7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="O7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="P7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="Q7" s="30" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -6521,19 +6518,19 @@
         <v>239</v>
       </c>
       <c r="L8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="M8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="O8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q8" s="30" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -6568,19 +6565,19 @@
         <v>239</v>
       </c>
       <c r="L9" t="s">
+        <v>359</v>
+      </c>
+      <c r="M9" t="s">
+        <v>387</v>
+      </c>
+      <c r="O9" t="s">
         <v>360</v>
       </c>
-      <c r="M9" t="s">
-        <v>388</v>
-      </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>361</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" s="30" t="s">
         <v>362</v>
-      </c>
-      <c r="Q9" s="30" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -6615,19 +6612,19 @@
         <v>239</v>
       </c>
       <c r="L10" t="s">
+        <v>363</v>
+      </c>
+      <c r="M10" t="s">
+        <v>388</v>
+      </c>
+      <c r="O10" t="s">
         <v>364</v>
       </c>
-      <c r="M10" t="s">
-        <v>389</v>
-      </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>365</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" s="30" t="s">
         <v>366</v>
-      </c>
-      <c r="Q10" s="30" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -6662,19 +6659,19 @@
         <v>239</v>
       </c>
       <c r="L11" t="s">
+        <v>378</v>
+      </c>
+      <c r="M11" t="s">
+        <v>389</v>
+      </c>
+      <c r="O11" t="s">
         <v>379</v>
       </c>
-      <c r="M11" t="s">
-        <v>390</v>
-      </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>380</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" s="23" t="s">
         <v>381</v>
-      </c>
-      <c r="Q11" s="23" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -6693,18 +6690,18 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B17" s="27"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="27" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -6714,22 +6711,22 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="27" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="27" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="27" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -6742,8 +6739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -6816,8 +6813,8 @@
       <c r="C2" t="s">
         <v>230</v>
       </c>
-      <c r="D2" t="s">
-        <v>308</v>
+      <c r="D2" s="27" t="s">
+        <v>253</v>
       </c>
       <c r="E2">
         <v>30</v>
@@ -6838,19 +6835,19 @@
         <v>239</v>
       </c>
       <c r="M2" t="s">
+        <v>432</v>
+      </c>
+      <c r="N2" t="s">
         <v>433</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>434</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>435</v>
       </c>
-      <c r="Q2" t="s">
-        <v>436</v>
-      </c>
       <c r="R2" s="23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -6863,8 +6860,8 @@
       <c r="C3" t="s">
         <v>212</v>
       </c>
-      <c r="D3" t="s">
-        <v>308</v>
+      <c r="D3" s="27" t="s">
+        <v>253</v>
       </c>
       <c r="E3">
         <v>60</v>
@@ -6886,19 +6883,19 @@
         <v>239</v>
       </c>
       <c r="M3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="N3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="P3" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q3" t="s">
         <v>424</v>
       </c>
-      <c r="Q3" t="s">
-        <v>425</v>
-      </c>
       <c r="R3" s="28" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -6911,8 +6908,8 @@
       <c r="C4" t="s">
         <v>230</v>
       </c>
-      <c r="D4" t="s">
-        <v>308</v>
+      <c r="D4" s="27" t="s">
+        <v>253</v>
       </c>
       <c r="E4">
         <v>20</v>
@@ -6933,19 +6930,19 @@
         <v>239</v>
       </c>
       <c r="M4" t="s">
+        <v>436</v>
+      </c>
+      <c r="N4" t="s">
         <v>437</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>438</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>439</v>
       </c>
-      <c r="Q4" t="s">
-        <v>440</v>
-      </c>
       <c r="R4" s="28" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -6980,19 +6977,19 @@
         <v>239</v>
       </c>
       <c r="M5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="N5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="P5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="R5" s="23" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -7027,19 +7024,19 @@
         <v>239</v>
       </c>
       <c r="M6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="N6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="P6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Q6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R6" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
@@ -7074,19 +7071,19 @@
         <v>239</v>
       </c>
       <c r="M7" t="s">
+        <v>406</v>
+      </c>
+      <c r="N7" t="s">
+        <v>430</v>
+      </c>
+      <c r="P7" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q7" t="s">
         <v>407</v>
       </c>
-      <c r="N7" t="s">
-        <v>431</v>
-      </c>
-      <c r="P7" t="s">
-        <v>411</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>408</v>
-      </c>
       <c r="R7" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -7121,19 +7118,19 @@
         <v>239</v>
       </c>
       <c r="M8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="N8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="P8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="R8" s="28" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
@@ -7146,8 +7143,8 @@
       <c r="C9" t="s">
         <v>227</v>
       </c>
-      <c r="D9" t="s">
-        <v>308</v>
+      <c r="D9" s="27" t="s">
+        <v>253</v>
       </c>
       <c r="E9">
         <v>28</v>
@@ -7168,19 +7165,19 @@
         <v>239</v>
       </c>
       <c r="M9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="N9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="P9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="Q9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="R9" s="23" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -7193,8 +7190,8 @@
       <c r="C10" t="s">
         <v>227</v>
       </c>
-      <c r="D10" t="s">
-        <v>308</v>
+      <c r="D10" s="27" t="s">
+        <v>253</v>
       </c>
       <c r="E10">
         <v>35</v>
@@ -7215,19 +7212,19 @@
         <v>239</v>
       </c>
       <c r="M10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="N10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="P10" t="s">
+        <v>445</v>
+      </c>
+      <c r="Q10" t="s">
         <v>446</v>
       </c>
-      <c r="Q10" t="s">
-        <v>447</v>
-      </c>
       <c r="R10" s="23" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -7240,8 +7237,8 @@
       <c r="C11" t="s">
         <v>212</v>
       </c>
-      <c r="D11" t="s">
-        <v>308</v>
+      <c r="D11" s="27" t="s">
+        <v>253</v>
       </c>
       <c r="E11">
         <v>30</v>
@@ -7262,24 +7259,24 @@
         <v>239</v>
       </c>
       <c r="M11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="N11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="P11" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="R11" s="28" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="N12" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -7294,18 +7291,18 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B17" s="27"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="27" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -7315,17 +7312,17 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="27" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="27" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>